<commit_message>
Add field order to task, and field frozen to contest
</commit_message>
<xml_diff>
--- a/trans/initial_data/initial_data.xlsx
+++ b/trans/initial_data/initial_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="378">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -1057,6 +1057,9 @@
     <t xml:space="preserve">Uzbek</t>
   </si>
   <si>
+    <t xml:space="preserve">This sheet contains data imported separately by command loaddata, and is not used by command initialize.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Languages</t>
   </si>
   <si>
@@ -1072,6 +1075,9 @@
     <t xml:space="preserve">ISC</t>
   </si>
   <si>
+    <t xml:space="preserve">TST</t>
+  </si>
+  <si>
     <t xml:space="preserve">Users</t>
   </si>
   <si>
@@ -1102,6 +1108,9 @@
     <t xml:space="preserve">Sandbox</t>
   </si>
   <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
     <t xml:space="preserve">staff</t>
   </si>
   <si>
@@ -1111,16 +1120,16 @@
     <t xml:space="preserve">Practice</t>
   </si>
   <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
     <t xml:space="preserve">backup</t>
   </si>
   <si>
     <t xml:space="preserve">Backup</t>
   </si>
   <si>
-    <t xml:space="preserve">LTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TST</t>
+    <t xml:space="preserve">Test</t>
   </si>
   <si>
     <t xml:space="preserve">day1</t>
@@ -1154,9 +1163,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1312,6 +1322,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1380,20 +1398,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1491,7 +1501,7 @@
   </sheetPr>
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -3952,7 +3962,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="4" style="4" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="257" style="5" width="16.29"/>
@@ -4680,8 +4690,8 @@
   </sheetPr>
   <dimension ref="A1:IW1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4693,282 +4703,274 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="254" style="5" width="16.29"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="true" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="12" customFormat="true" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="11" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11"/>
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11"/>
+      <c r="BN1" s="11"/>
+      <c r="BO1" s="11"/>
+      <c r="BP1" s="11"/>
+      <c r="BQ1" s="11"/>
+      <c r="BR1" s="11"/>
+      <c r="BS1" s="11"/>
+      <c r="BT1" s="11"/>
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11"/>
+      <c r="CA1" s="11"/>
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11"/>
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11"/>
+      <c r="CI1" s="11"/>
+      <c r="CJ1" s="11"/>
+      <c r="CK1" s="11"/>
+      <c r="CL1" s="11"/>
+      <c r="CM1" s="11"/>
+      <c r="CN1" s="11"/>
+      <c r="CO1" s="11"/>
+      <c r="CP1" s="11"/>
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11"/>
+      <c r="CW1" s="11"/>
+      <c r="CX1" s="11"/>
+      <c r="CY1" s="11"/>
+      <c r="CZ1" s="11"/>
+      <c r="DA1" s="11"/>
+      <c r="DB1" s="11"/>
+      <c r="DC1" s="11"/>
+      <c r="DD1" s="11"/>
+      <c r="DE1" s="11"/>
+      <c r="DF1" s="11"/>
+      <c r="DG1" s="11"/>
+      <c r="DH1" s="11"/>
+      <c r="DI1" s="11"/>
+      <c r="DJ1" s="11"/>
+      <c r="DK1" s="11"/>
+      <c r="DL1" s="11"/>
+      <c r="DM1" s="11"/>
+      <c r="DN1" s="11"/>
+      <c r="DO1" s="11"/>
+      <c r="DP1" s="11"/>
+      <c r="DQ1" s="11"/>
+      <c r="DR1" s="11"/>
+      <c r="DS1" s="11"/>
+      <c r="DT1" s="11"/>
+      <c r="DU1" s="11"/>
+      <c r="DV1" s="11"/>
+      <c r="DW1" s="11"/>
+      <c r="DX1" s="11"/>
+      <c r="DY1" s="11"/>
+      <c r="DZ1" s="11"/>
+      <c r="EA1" s="11"/>
+      <c r="EB1" s="11"/>
+      <c r="EC1" s="11"/>
+      <c r="ED1" s="11"/>
+      <c r="EE1" s="11"/>
+      <c r="EF1" s="11"/>
+      <c r="EG1" s="11"/>
+      <c r="EH1" s="11"/>
+      <c r="EI1" s="11"/>
+      <c r="EJ1" s="11"/>
+      <c r="EK1" s="11"/>
+      <c r="EL1" s="11"/>
+      <c r="EM1" s="11"/>
+      <c r="EN1" s="11"/>
+      <c r="EO1" s="11"/>
+      <c r="EP1" s="11"/>
+      <c r="EQ1" s="11"/>
+      <c r="ER1" s="11"/>
+      <c r="ES1" s="11"/>
+      <c r="ET1" s="11"/>
+      <c r="EU1" s="11"/>
+      <c r="EV1" s="11"/>
+      <c r="EW1" s="11"/>
+      <c r="EX1" s="11"/>
+      <c r="EY1" s="11"/>
+      <c r="EZ1" s="11"/>
+      <c r="FA1" s="11"/>
+      <c r="FB1" s="11"/>
+      <c r="FC1" s="11"/>
+      <c r="FD1" s="11"/>
+      <c r="FE1" s="11"/>
+      <c r="FF1" s="11"/>
+      <c r="FG1" s="11"/>
+      <c r="FH1" s="11"/>
+      <c r="FI1" s="11"/>
+      <c r="FJ1" s="11"/>
+      <c r="FK1" s="11"/>
+      <c r="FL1" s="11"/>
+      <c r="FM1" s="11"/>
+      <c r="FN1" s="11"/>
+      <c r="FO1" s="11"/>
+      <c r="FP1" s="11"/>
+      <c r="FQ1" s="11"/>
+      <c r="FR1" s="11"/>
+      <c r="FS1" s="11"/>
+      <c r="FT1" s="11"/>
+      <c r="FU1" s="11"/>
+      <c r="FV1" s="11"/>
+      <c r="FW1" s="11"/>
+      <c r="FX1" s="11"/>
+      <c r="FY1" s="11"/>
+      <c r="FZ1" s="11"/>
+      <c r="GA1" s="11"/>
+      <c r="GB1" s="11"/>
+      <c r="GC1" s="11"/>
+      <c r="GD1" s="11"/>
+      <c r="GE1" s="11"/>
+      <c r="GF1" s="11"/>
+      <c r="GG1" s="11"/>
+      <c r="GH1" s="11"/>
+      <c r="GI1" s="11"/>
+      <c r="GJ1" s="11"/>
+      <c r="GK1" s="11"/>
+      <c r="GL1" s="11"/>
+      <c r="GM1" s="11"/>
+      <c r="GN1" s="11"/>
+      <c r="GO1" s="11"/>
+      <c r="GP1" s="11"/>
+      <c r="GQ1" s="11"/>
+      <c r="GR1" s="11"/>
+      <c r="GS1" s="11"/>
+      <c r="GT1" s="11"/>
+      <c r="GU1" s="11"/>
+      <c r="GV1" s="11"/>
+      <c r="GW1" s="11"/>
+      <c r="GX1" s="11"/>
+      <c r="GY1" s="11"/>
+      <c r="GZ1" s="11"/>
+      <c r="HA1" s="11"/>
+      <c r="HB1" s="11"/>
+      <c r="HC1" s="11"/>
+      <c r="HD1" s="11"/>
+      <c r="HE1" s="11"/>
+      <c r="HF1" s="11"/>
+      <c r="HG1" s="11"/>
+      <c r="HH1" s="11"/>
+      <c r="HI1" s="11"/>
+      <c r="HJ1" s="11"/>
+      <c r="HK1" s="11"/>
+      <c r="HL1" s="11"/>
+      <c r="HM1" s="11"/>
+      <c r="HN1" s="11"/>
+      <c r="HO1" s="11"/>
+      <c r="HP1" s="11"/>
+      <c r="HQ1" s="11"/>
+      <c r="HR1" s="11"/>
+      <c r="HS1" s="11"/>
+      <c r="HT1" s="11"/>
+      <c r="HU1" s="11"/>
+      <c r="HV1" s="11"/>
+      <c r="HW1" s="11"/>
+      <c r="HX1" s="11"/>
+      <c r="HY1" s="11"/>
+      <c r="HZ1" s="11"/>
+      <c r="IA1" s="11"/>
+      <c r="IB1" s="11"/>
+      <c r="IC1" s="11"/>
+      <c r="ID1" s="11"/>
+      <c r="IE1" s="11"/>
+      <c r="IF1" s="11"/>
+      <c r="IG1" s="11"/>
+      <c r="IH1" s="11"/>
+      <c r="II1" s="11"/>
+      <c r="IJ1" s="11"/>
+      <c r="IK1" s="11"/>
+      <c r="IL1" s="11"/>
+      <c r="IM1" s="11"/>
+      <c r="IN1" s="11"/>
+      <c r="IO1" s="11"/>
+      <c r="IP1" s="11"/>
+      <c r="IQ1" s="11"/>
+      <c r="IR1" s="11"/>
+      <c r="IS1" s="11"/>
+    </row>
+    <row r="2" s="15" customFormat="true" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12"/>
-      <c r="BL1" s="12"/>
-      <c r="BM1" s="12"/>
-      <c r="BN1" s="12"/>
-      <c r="BO1" s="12"/>
-      <c r="BP1" s="12"/>
-      <c r="BQ1" s="12"/>
-      <c r="BR1" s="12"/>
-      <c r="BS1" s="12"/>
-      <c r="BT1" s="12"/>
-      <c r="BU1" s="12"/>
-      <c r="BV1" s="12"/>
-      <c r="BW1" s="12"/>
-      <c r="BX1" s="12"/>
-      <c r="BY1" s="12"/>
-      <c r="BZ1" s="12"/>
-      <c r="CA1" s="12"/>
-      <c r="CB1" s="12"/>
-      <c r="CC1" s="12"/>
-      <c r="CD1" s="12"/>
-      <c r="CE1" s="12"/>
-      <c r="CF1" s="12"/>
-      <c r="CG1" s="12"/>
-      <c r="CH1" s="12"/>
-      <c r="CI1" s="12"/>
-      <c r="CJ1" s="12"/>
-      <c r="CK1" s="12"/>
-      <c r="CL1" s="12"/>
-      <c r="CM1" s="12"/>
-      <c r="CN1" s="12"/>
-      <c r="CO1" s="12"/>
-      <c r="CP1" s="12"/>
-      <c r="CQ1" s="12"/>
-      <c r="CR1" s="12"/>
-      <c r="CS1" s="12"/>
-      <c r="CT1" s="12"/>
-      <c r="CU1" s="12"/>
-      <c r="CV1" s="12"/>
-      <c r="CW1" s="12"/>
-      <c r="CX1" s="12"/>
-      <c r="CY1" s="12"/>
-      <c r="CZ1" s="12"/>
-      <c r="DA1" s="12"/>
-      <c r="DB1" s="12"/>
-      <c r="DC1" s="12"/>
-      <c r="DD1" s="12"/>
-      <c r="DE1" s="12"/>
-      <c r="DF1" s="12"/>
-      <c r="DG1" s="12"/>
-      <c r="DH1" s="12"/>
-      <c r="DI1" s="12"/>
-      <c r="DJ1" s="12"/>
-      <c r="DK1" s="12"/>
-      <c r="DL1" s="12"/>
-      <c r="DM1" s="12"/>
-      <c r="DN1" s="12"/>
-      <c r="DO1" s="12"/>
-      <c r="DP1" s="12"/>
-      <c r="DQ1" s="12"/>
-      <c r="DR1" s="12"/>
-      <c r="DS1" s="12"/>
-      <c r="DT1" s="12"/>
-      <c r="DU1" s="12"/>
-      <c r="DV1" s="12"/>
-      <c r="DW1" s="12"/>
-      <c r="DX1" s="12"/>
-      <c r="DY1" s="12"/>
-      <c r="DZ1" s="12"/>
-      <c r="EA1" s="12"/>
-      <c r="EB1" s="12"/>
-      <c r="EC1" s="12"/>
-      <c r="ED1" s="12"/>
-      <c r="EE1" s="12"/>
-      <c r="EF1" s="12"/>
-      <c r="EG1" s="12"/>
-      <c r="EH1" s="12"/>
-      <c r="EI1" s="12"/>
-      <c r="EJ1" s="12"/>
-      <c r="EK1" s="12"/>
-      <c r="EL1" s="12"/>
-      <c r="EM1" s="12"/>
-      <c r="EN1" s="12"/>
-      <c r="EO1" s="12"/>
-      <c r="EP1" s="12"/>
-      <c r="EQ1" s="12"/>
-      <c r="ER1" s="12"/>
-      <c r="ES1" s="12"/>
-      <c r="ET1" s="12"/>
-      <c r="EU1" s="12"/>
-      <c r="EV1" s="12"/>
-      <c r="EW1" s="12"/>
-      <c r="EX1" s="12"/>
-      <c r="EY1" s="12"/>
-      <c r="EZ1" s="12"/>
-      <c r="FA1" s="12"/>
-      <c r="FB1" s="12"/>
-      <c r="FC1" s="12"/>
-      <c r="FD1" s="12"/>
-      <c r="FE1" s="12"/>
-      <c r="FF1" s="12"/>
-      <c r="FG1" s="12"/>
-      <c r="FH1" s="12"/>
-      <c r="FI1" s="12"/>
-      <c r="FJ1" s="12"/>
-      <c r="FK1" s="12"/>
-      <c r="FL1" s="12"/>
-      <c r="FM1" s="12"/>
-      <c r="FN1" s="12"/>
-      <c r="FO1" s="12"/>
-      <c r="FP1" s="12"/>
-      <c r="FQ1" s="12"/>
-      <c r="FR1" s="12"/>
-      <c r="FS1" s="12"/>
-      <c r="FT1" s="12"/>
-      <c r="FU1" s="12"/>
-      <c r="FV1" s="12"/>
-      <c r="FW1" s="12"/>
-      <c r="FX1" s="12"/>
-      <c r="FY1" s="12"/>
-      <c r="FZ1" s="12"/>
-      <c r="GA1" s="12"/>
-      <c r="GB1" s="12"/>
-      <c r="GC1" s="12"/>
-      <c r="GD1" s="12"/>
-      <c r="GE1" s="12"/>
-      <c r="GF1" s="12"/>
-      <c r="GG1" s="12"/>
-      <c r="GH1" s="12"/>
-      <c r="GI1" s="12"/>
-      <c r="GJ1" s="12"/>
-      <c r="GK1" s="12"/>
-      <c r="GL1" s="12"/>
-      <c r="GM1" s="12"/>
-      <c r="GN1" s="12"/>
-      <c r="GO1" s="12"/>
-      <c r="GP1" s="12"/>
-      <c r="GQ1" s="12"/>
-      <c r="GR1" s="12"/>
-      <c r="GS1" s="12"/>
-      <c r="GT1" s="12"/>
-      <c r="GU1" s="12"/>
-      <c r="GV1" s="12"/>
-      <c r="GW1" s="12"/>
-      <c r="GX1" s="12"/>
-      <c r="GY1" s="12"/>
-      <c r="GZ1" s="12"/>
-      <c r="HA1" s="12"/>
-      <c r="HB1" s="12"/>
-      <c r="HC1" s="12"/>
-      <c r="HD1" s="12"/>
-      <c r="HE1" s="12"/>
-      <c r="HF1" s="12"/>
-      <c r="HG1" s="12"/>
-      <c r="HH1" s="12"/>
-      <c r="HI1" s="12"/>
-      <c r="HJ1" s="12"/>
-      <c r="HK1" s="12"/>
-      <c r="HL1" s="12"/>
-      <c r="HM1" s="12"/>
-      <c r="HN1" s="12"/>
-      <c r="HO1" s="12"/>
-      <c r="HP1" s="12"/>
-      <c r="HQ1" s="12"/>
-      <c r="HR1" s="12"/>
-      <c r="HS1" s="12"/>
-      <c r="HT1" s="12"/>
-      <c r="HU1" s="12"/>
-      <c r="HV1" s="12"/>
-      <c r="HW1" s="12"/>
-      <c r="HX1" s="12"/>
-      <c r="HY1" s="12"/>
-      <c r="HZ1" s="12"/>
-      <c r="IA1" s="12"/>
-      <c r="IB1" s="12"/>
-      <c r="IC1" s="12"/>
-      <c r="ID1" s="12"/>
-      <c r="IE1" s="12"/>
-      <c r="IF1" s="12"/>
-      <c r="IG1" s="12"/>
-      <c r="IH1" s="12"/>
-      <c r="II1" s="12"/>
-      <c r="IJ1" s="12"/>
-      <c r="IK1" s="12"/>
-      <c r="IL1" s="12"/>
-      <c r="IM1" s="12"/>
-      <c r="IN1" s="12"/>
-      <c r="IO1" s="12"/>
-      <c r="IP1" s="12"/>
-      <c r="IQ1" s="12"/>
-      <c r="IR1" s="12"/>
-      <c r="IS1" s="12"/>
-    </row>
-    <row r="2" s="16" customFormat="true" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>130</v>
-      </c>
+      <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -5217,35 +5219,282 @@
       <c r="IR2" s="14"/>
       <c r="IS2" s="14"/>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+    <row r="3" s="18" customFormat="true" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="16"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="16"/>
+      <c r="AN3" s="16"/>
+      <c r="AO3" s="16"/>
+      <c r="AP3" s="16"/>
+      <c r="AQ3" s="16"/>
+      <c r="AR3" s="16"/>
+      <c r="AS3" s="16"/>
+      <c r="AT3" s="16"/>
+      <c r="AU3" s="16"/>
+      <c r="AV3" s="16"/>
+      <c r="AW3" s="16"/>
+      <c r="AX3" s="16"/>
+      <c r="AY3" s="16"/>
+      <c r="AZ3" s="16"/>
+      <c r="BA3" s="16"/>
+      <c r="BB3" s="16"/>
+      <c r="BC3" s="16"/>
+      <c r="BD3" s="16"/>
+      <c r="BE3" s="16"/>
+      <c r="BF3" s="16"/>
+      <c r="BG3" s="16"/>
+      <c r="BH3" s="16"/>
+      <c r="BI3" s="16"/>
+      <c r="BJ3" s="16"/>
+      <c r="BK3" s="16"/>
+      <c r="BL3" s="16"/>
+      <c r="BM3" s="16"/>
+      <c r="BN3" s="16"/>
+      <c r="BO3" s="16"/>
+      <c r="BP3" s="16"/>
+      <c r="BQ3" s="16"/>
+      <c r="BR3" s="16"/>
+      <c r="BS3" s="16"/>
+      <c r="BT3" s="16"/>
+      <c r="BU3" s="16"/>
+      <c r="BV3" s="16"/>
+      <c r="BW3" s="16"/>
+      <c r="BX3" s="16"/>
+      <c r="BY3" s="16"/>
+      <c r="BZ3" s="16"/>
+      <c r="CA3" s="16"/>
+      <c r="CB3" s="16"/>
+      <c r="CC3" s="16"/>
+      <c r="CD3" s="16"/>
+      <c r="CE3" s="16"/>
+      <c r="CF3" s="16"/>
+      <c r="CG3" s="16"/>
+      <c r="CH3" s="16"/>
+      <c r="CI3" s="16"/>
+      <c r="CJ3" s="16"/>
+      <c r="CK3" s="16"/>
+      <c r="CL3" s="16"/>
+      <c r="CM3" s="16"/>
+      <c r="CN3" s="16"/>
+      <c r="CO3" s="16"/>
+      <c r="CP3" s="16"/>
+      <c r="CQ3" s="16"/>
+      <c r="CR3" s="16"/>
+      <c r="CS3" s="16"/>
+      <c r="CT3" s="16"/>
+      <c r="CU3" s="16"/>
+      <c r="CV3" s="16"/>
+      <c r="CW3" s="16"/>
+      <c r="CX3" s="16"/>
+      <c r="CY3" s="16"/>
+      <c r="CZ3" s="16"/>
+      <c r="DA3" s="16"/>
+      <c r="DB3" s="16"/>
+      <c r="DC3" s="16"/>
+      <c r="DD3" s="16"/>
+      <c r="DE3" s="16"/>
+      <c r="DF3" s="16"/>
+      <c r="DG3" s="16"/>
+      <c r="DH3" s="16"/>
+      <c r="DI3" s="16"/>
+      <c r="DJ3" s="16"/>
+      <c r="DK3" s="16"/>
+      <c r="DL3" s="16"/>
+      <c r="DM3" s="16"/>
+      <c r="DN3" s="16"/>
+      <c r="DO3" s="16"/>
+      <c r="DP3" s="16"/>
+      <c r="DQ3" s="16"/>
+      <c r="DR3" s="16"/>
+      <c r="DS3" s="16"/>
+      <c r="DT3" s="16"/>
+      <c r="DU3" s="16"/>
+      <c r="DV3" s="16"/>
+      <c r="DW3" s="16"/>
+      <c r="DX3" s="16"/>
+      <c r="DY3" s="16"/>
+      <c r="DZ3" s="16"/>
+      <c r="EA3" s="16"/>
+      <c r="EB3" s="16"/>
+      <c r="EC3" s="16"/>
+      <c r="ED3" s="16"/>
+      <c r="EE3" s="16"/>
+      <c r="EF3" s="16"/>
+      <c r="EG3" s="16"/>
+      <c r="EH3" s="16"/>
+      <c r="EI3" s="16"/>
+      <c r="EJ3" s="16"/>
+      <c r="EK3" s="16"/>
+      <c r="EL3" s="16"/>
+      <c r="EM3" s="16"/>
+      <c r="EN3" s="16"/>
+      <c r="EO3" s="16"/>
+      <c r="EP3" s="16"/>
+      <c r="EQ3" s="16"/>
+      <c r="ER3" s="16"/>
+      <c r="ES3" s="16"/>
+      <c r="ET3" s="16"/>
+      <c r="EU3" s="16"/>
+      <c r="EV3" s="16"/>
+      <c r="EW3" s="16"/>
+      <c r="EX3" s="16"/>
+      <c r="EY3" s="16"/>
+      <c r="EZ3" s="16"/>
+      <c r="FA3" s="16"/>
+      <c r="FB3" s="16"/>
+      <c r="FC3" s="16"/>
+      <c r="FD3" s="16"/>
+      <c r="FE3" s="16"/>
+      <c r="FF3" s="16"/>
+      <c r="FG3" s="16"/>
+      <c r="FH3" s="16"/>
+      <c r="FI3" s="16"/>
+      <c r="FJ3" s="16"/>
+      <c r="FK3" s="16"/>
+      <c r="FL3" s="16"/>
+      <c r="FM3" s="16"/>
+      <c r="FN3" s="16"/>
+      <c r="FO3" s="16"/>
+      <c r="FP3" s="16"/>
+      <c r="FQ3" s="16"/>
+      <c r="FR3" s="16"/>
+      <c r="FS3" s="16"/>
+      <c r="FT3" s="16"/>
+      <c r="FU3" s="16"/>
+      <c r="FV3" s="16"/>
+      <c r="FW3" s="16"/>
+      <c r="FX3" s="16"/>
+      <c r="FY3" s="16"/>
+      <c r="FZ3" s="16"/>
+      <c r="GA3" s="16"/>
+      <c r="GB3" s="16"/>
+      <c r="GC3" s="16"/>
+      <c r="GD3" s="16"/>
+      <c r="GE3" s="16"/>
+      <c r="GF3" s="16"/>
+      <c r="GG3" s="16"/>
+      <c r="GH3" s="16"/>
+      <c r="GI3" s="16"/>
+      <c r="GJ3" s="16"/>
+      <c r="GK3" s="16"/>
+      <c r="GL3" s="16"/>
+      <c r="GM3" s="16"/>
+      <c r="GN3" s="16"/>
+      <c r="GO3" s="16"/>
+      <c r="GP3" s="16"/>
+      <c r="GQ3" s="16"/>
+      <c r="GR3" s="16"/>
+      <c r="GS3" s="16"/>
+      <c r="GT3" s="16"/>
+      <c r="GU3" s="16"/>
+      <c r="GV3" s="16"/>
+      <c r="GW3" s="16"/>
+      <c r="GX3" s="16"/>
+      <c r="GY3" s="16"/>
+      <c r="GZ3" s="16"/>
+      <c r="HA3" s="16"/>
+      <c r="HB3" s="16"/>
+      <c r="HC3" s="16"/>
+      <c r="HD3" s="16"/>
+      <c r="HE3" s="16"/>
+      <c r="HF3" s="16"/>
+      <c r="HG3" s="16"/>
+      <c r="HH3" s="16"/>
+      <c r="HI3" s="16"/>
+      <c r="HJ3" s="16"/>
+      <c r="HK3" s="16"/>
+      <c r="HL3" s="16"/>
+      <c r="HM3" s="16"/>
+      <c r="HN3" s="16"/>
+      <c r="HO3" s="16"/>
+      <c r="HP3" s="16"/>
+      <c r="HQ3" s="16"/>
+      <c r="HR3" s="16"/>
+      <c r="HS3" s="16"/>
+      <c r="HT3" s="16"/>
+      <c r="HU3" s="16"/>
+      <c r="HV3" s="16"/>
+      <c r="HW3" s="16"/>
+      <c r="HX3" s="16"/>
+      <c r="HY3" s="16"/>
+      <c r="HZ3" s="16"/>
+      <c r="IA3" s="16"/>
+      <c r="IB3" s="16"/>
+      <c r="IC3" s="16"/>
+      <c r="ID3" s="16"/>
+      <c r="IE3" s="16"/>
+      <c r="IF3" s="16"/>
+      <c r="IG3" s="16"/>
+      <c r="IH3" s="16"/>
+      <c r="II3" s="16"/>
+      <c r="IJ3" s="16"/>
+      <c r="IK3" s="16"/>
+      <c r="IL3" s="16"/>
+      <c r="IM3" s="16"/>
+      <c r="IN3" s="16"/>
+      <c r="IO3" s="16"/>
+      <c r="IP3" s="16"/>
+      <c r="IQ3" s="16"/>
+      <c r="IR3" s="16"/>
+      <c r="IS3" s="16"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="4" t="s">
         <v>348</v>
       </c>
@@ -5254,567 +5503,589 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D5" s="17"/>
+      <c r="A5" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D6" s="17"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" s="13" customFormat="true" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
-        <v>349</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="18" t="s">
+      <c r="D6" s="19"/>
+      <c r="E6" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="F6" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" s="15" customFormat="true" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="20" t="s">
+        <v>352</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="12"/>
-      <c r="AB8" s="12"/>
-      <c r="AC8" s="12"/>
-      <c r="AD8" s="12"/>
-      <c r="AE8" s="12"/>
-      <c r="AF8" s="12"/>
-      <c r="AG8" s="12"/>
-      <c r="AH8" s="12"/>
-      <c r="AI8" s="12"/>
-      <c r="AJ8" s="12"/>
-      <c r="AK8" s="12"/>
-      <c r="AL8" s="12"/>
-      <c r="AM8" s="12"/>
-      <c r="AN8" s="12"/>
-      <c r="AO8" s="12"/>
-      <c r="AP8" s="12"/>
-      <c r="AQ8" s="12"/>
-      <c r="AR8" s="12"/>
-      <c r="AS8" s="12"/>
-      <c r="AT8" s="12"/>
-      <c r="AU8" s="12"/>
-      <c r="AV8" s="12"/>
-      <c r="AW8" s="12"/>
-      <c r="AX8" s="12"/>
-      <c r="AY8" s="12"/>
-      <c r="AZ8" s="12"/>
-      <c r="BA8" s="12"/>
-      <c r="BB8" s="12"/>
-      <c r="BC8" s="12"/>
-      <c r="BD8" s="12"/>
-      <c r="BE8" s="12"/>
-      <c r="BF8" s="12"/>
-      <c r="BG8" s="12"/>
-      <c r="BH8" s="12"/>
-      <c r="BI8" s="12"/>
-      <c r="BJ8" s="12"/>
-      <c r="BK8" s="12"/>
-      <c r="BL8" s="12"/>
-      <c r="BM8" s="12"/>
-      <c r="BN8" s="12"/>
-      <c r="BO8" s="12"/>
-      <c r="BP8" s="12"/>
-      <c r="BQ8" s="12"/>
-      <c r="BR8" s="12"/>
-      <c r="BS8" s="12"/>
-      <c r="BT8" s="12"/>
-      <c r="BU8" s="12"/>
-      <c r="BV8" s="12"/>
-      <c r="BW8" s="12"/>
-      <c r="BX8" s="12"/>
-      <c r="BY8" s="12"/>
-      <c r="BZ8" s="12"/>
-      <c r="CA8" s="12"/>
-      <c r="CB8" s="12"/>
-      <c r="CC8" s="12"/>
-      <c r="CD8" s="12"/>
-      <c r="CE8" s="12"/>
-      <c r="CF8" s="12"/>
-      <c r="CG8" s="12"/>
-      <c r="CH8" s="12"/>
-      <c r="CI8" s="12"/>
-      <c r="CJ8" s="12"/>
-      <c r="CK8" s="12"/>
-      <c r="CL8" s="12"/>
-      <c r="CM8" s="12"/>
-      <c r="CN8" s="12"/>
-      <c r="CO8" s="12"/>
-      <c r="CP8" s="12"/>
-      <c r="CQ8" s="12"/>
-      <c r="CR8" s="12"/>
-      <c r="CS8" s="12"/>
-      <c r="CT8" s="12"/>
-      <c r="CU8" s="12"/>
-      <c r="CV8" s="12"/>
-      <c r="CW8" s="12"/>
-      <c r="CX8" s="12"/>
-      <c r="CY8" s="12"/>
-      <c r="CZ8" s="12"/>
-      <c r="DA8" s="12"/>
-      <c r="DB8" s="12"/>
-      <c r="DC8" s="12"/>
-      <c r="DD8" s="12"/>
-      <c r="DE8" s="12"/>
-      <c r="DF8" s="12"/>
-      <c r="DG8" s="12"/>
-      <c r="DH8" s="12"/>
-      <c r="DI8" s="12"/>
-      <c r="DJ8" s="12"/>
-      <c r="DK8" s="12"/>
-      <c r="DL8" s="12"/>
-      <c r="DM8" s="12"/>
-      <c r="DN8" s="12"/>
-      <c r="DO8" s="12"/>
-      <c r="DP8" s="12"/>
-      <c r="DQ8" s="12"/>
-      <c r="DR8" s="12"/>
-      <c r="DS8" s="12"/>
-      <c r="DT8" s="12"/>
-      <c r="DU8" s="12"/>
-      <c r="DV8" s="12"/>
-      <c r="DW8" s="12"/>
-      <c r="DX8" s="12"/>
-      <c r="DY8" s="12"/>
-      <c r="DZ8" s="12"/>
-      <c r="EA8" s="12"/>
-      <c r="EB8" s="12"/>
-      <c r="EC8" s="12"/>
-      <c r="ED8" s="12"/>
-      <c r="EE8" s="12"/>
-      <c r="EF8" s="12"/>
-      <c r="EG8" s="12"/>
-      <c r="EH8" s="12"/>
-      <c r="EI8" s="12"/>
-      <c r="EJ8" s="12"/>
-      <c r="EK8" s="12"/>
-      <c r="EL8" s="12"/>
-      <c r="EM8" s="12"/>
-      <c r="EN8" s="12"/>
-      <c r="EO8" s="12"/>
-      <c r="EP8" s="12"/>
-      <c r="EQ8" s="12"/>
-      <c r="ER8" s="12"/>
-      <c r="ES8" s="12"/>
-      <c r="ET8" s="12"/>
-      <c r="EU8" s="12"/>
-      <c r="EV8" s="12"/>
-      <c r="EW8" s="12"/>
-      <c r="EX8" s="12"/>
-      <c r="EY8" s="12"/>
-      <c r="EZ8" s="12"/>
-      <c r="FA8" s="12"/>
-      <c r="FB8" s="12"/>
-      <c r="FC8" s="12"/>
-      <c r="FD8" s="12"/>
-      <c r="FE8" s="12"/>
-      <c r="FF8" s="12"/>
-      <c r="FG8" s="12"/>
-      <c r="FH8" s="12"/>
-      <c r="FI8" s="12"/>
-      <c r="FJ8" s="12"/>
-      <c r="FK8" s="12"/>
-      <c r="FL8" s="12"/>
-      <c r="FM8" s="12"/>
-      <c r="FN8" s="12"/>
-      <c r="FO8" s="12"/>
-      <c r="FP8" s="12"/>
-      <c r="FQ8" s="12"/>
-      <c r="FR8" s="12"/>
-      <c r="FS8" s="12"/>
-      <c r="FT8" s="12"/>
-      <c r="FU8" s="12"/>
-      <c r="FV8" s="12"/>
-      <c r="FW8" s="12"/>
-      <c r="FX8" s="12"/>
-      <c r="FY8" s="12"/>
-      <c r="FZ8" s="12"/>
-      <c r="GA8" s="12"/>
-      <c r="GB8" s="12"/>
-      <c r="GC8" s="12"/>
-      <c r="GD8" s="12"/>
-      <c r="GE8" s="12"/>
-      <c r="GF8" s="12"/>
-      <c r="GG8" s="12"/>
-      <c r="GH8" s="12"/>
-      <c r="GI8" s="12"/>
-      <c r="GJ8" s="12"/>
-      <c r="GK8" s="12"/>
-      <c r="GL8" s="12"/>
-      <c r="GM8" s="12"/>
-      <c r="GN8" s="12"/>
-      <c r="GO8" s="12"/>
-      <c r="GP8" s="12"/>
-      <c r="GQ8" s="12"/>
-      <c r="GR8" s="12"/>
-      <c r="GS8" s="12"/>
-      <c r="GT8" s="12"/>
-      <c r="GU8" s="12"/>
-      <c r="GV8" s="12"/>
-      <c r="GW8" s="12"/>
-      <c r="GX8" s="12"/>
-      <c r="GY8" s="12"/>
-      <c r="GZ8" s="12"/>
-      <c r="HA8" s="12"/>
-      <c r="HB8" s="12"/>
-      <c r="HC8" s="12"/>
-      <c r="HD8" s="12"/>
-      <c r="HE8" s="12"/>
-      <c r="HF8" s="12"/>
-      <c r="HG8" s="12"/>
-      <c r="HH8" s="12"/>
-      <c r="HI8" s="12"/>
-      <c r="HJ8" s="12"/>
-      <c r="HK8" s="12"/>
-      <c r="HL8" s="12"/>
-      <c r="HM8" s="12"/>
-      <c r="HN8" s="12"/>
-      <c r="HO8" s="12"/>
-      <c r="HP8" s="12"/>
-      <c r="HQ8" s="12"/>
-      <c r="HR8" s="12"/>
-      <c r="HS8" s="12"/>
-      <c r="HT8" s="12"/>
-      <c r="HU8" s="12"/>
-      <c r="HV8" s="12"/>
-      <c r="HW8" s="12"/>
-      <c r="HX8" s="12"/>
-      <c r="HY8" s="12"/>
-      <c r="HZ8" s="12"/>
-      <c r="IA8" s="12"/>
-      <c r="IB8" s="12"/>
-      <c r="IC8" s="12"/>
-      <c r="ID8" s="12"/>
-      <c r="IE8" s="12"/>
-      <c r="IF8" s="12"/>
-      <c r="IG8" s="12"/>
-      <c r="IH8" s="12"/>
-      <c r="II8" s="12"/>
-      <c r="IJ8" s="12"/>
-      <c r="IK8" s="12"/>
-      <c r="IL8" s="12"/>
-      <c r="IM8" s="12"/>
-      <c r="IN8" s="12"/>
-      <c r="IO8" s="12"/>
-      <c r="IP8" s="12"/>
-      <c r="IQ8" s="12"/>
-      <c r="IR8" s="12"/>
-      <c r="IS8" s="12"/>
-      <c r="IT8" s="12"/>
-      <c r="IU8" s="12"/>
-      <c r="IV8" s="12"/>
-      <c r="IW8" s="12"/>
-    </row>
-    <row r="9" s="16" customFormat="true" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="14"/>
+      <c r="AG8" s="14"/>
+      <c r="AH8" s="14"/>
+      <c r="AI8" s="14"/>
+      <c r="AJ8" s="14"/>
+      <c r="AK8" s="14"/>
+      <c r="AL8" s="14"/>
+      <c r="AM8" s="14"/>
+      <c r="AN8" s="14"/>
+      <c r="AO8" s="14"/>
+      <c r="AP8" s="14"/>
+      <c r="AQ8" s="14"/>
+      <c r="AR8" s="14"/>
+      <c r="AS8" s="14"/>
+      <c r="AT8" s="14"/>
+      <c r="AU8" s="14"/>
+      <c r="AV8" s="14"/>
+      <c r="AW8" s="14"/>
+      <c r="AX8" s="14"/>
+      <c r="AY8" s="14"/>
+      <c r="AZ8" s="14"/>
+      <c r="BA8" s="14"/>
+      <c r="BB8" s="14"/>
+      <c r="BC8" s="14"/>
+      <c r="BD8" s="14"/>
+      <c r="BE8" s="14"/>
+      <c r="BF8" s="14"/>
+      <c r="BG8" s="14"/>
+      <c r="BH8" s="14"/>
+      <c r="BI8" s="14"/>
+      <c r="BJ8" s="14"/>
+      <c r="BK8" s="14"/>
+      <c r="BL8" s="14"/>
+      <c r="BM8" s="14"/>
+      <c r="BN8" s="14"/>
+      <c r="BO8" s="14"/>
+      <c r="BP8" s="14"/>
+      <c r="BQ8" s="14"/>
+      <c r="BR8" s="14"/>
+      <c r="BS8" s="14"/>
+      <c r="BT8" s="14"/>
+      <c r="BU8" s="14"/>
+      <c r="BV8" s="14"/>
+      <c r="BW8" s="14"/>
+      <c r="BX8" s="14"/>
+      <c r="BY8" s="14"/>
+      <c r="BZ8" s="14"/>
+      <c r="CA8" s="14"/>
+      <c r="CB8" s="14"/>
+      <c r="CC8" s="14"/>
+      <c r="CD8" s="14"/>
+      <c r="CE8" s="14"/>
+      <c r="CF8" s="14"/>
+      <c r="CG8" s="14"/>
+      <c r="CH8" s="14"/>
+      <c r="CI8" s="14"/>
+      <c r="CJ8" s="14"/>
+      <c r="CK8" s="14"/>
+      <c r="CL8" s="14"/>
+      <c r="CM8" s="14"/>
+      <c r="CN8" s="14"/>
+      <c r="CO8" s="14"/>
+      <c r="CP8" s="14"/>
+      <c r="CQ8" s="14"/>
+      <c r="CR8" s="14"/>
+      <c r="CS8" s="14"/>
+      <c r="CT8" s="14"/>
+      <c r="CU8" s="14"/>
+      <c r="CV8" s="14"/>
+      <c r="CW8" s="14"/>
+      <c r="CX8" s="14"/>
+      <c r="CY8" s="14"/>
+      <c r="CZ8" s="14"/>
+      <c r="DA8" s="14"/>
+      <c r="DB8" s="14"/>
+      <c r="DC8" s="14"/>
+      <c r="DD8" s="14"/>
+      <c r="DE8" s="14"/>
+      <c r="DF8" s="14"/>
+      <c r="DG8" s="14"/>
+      <c r="DH8" s="14"/>
+      <c r="DI8" s="14"/>
+      <c r="DJ8" s="14"/>
+      <c r="DK8" s="14"/>
+      <c r="DL8" s="14"/>
+      <c r="DM8" s="14"/>
+      <c r="DN8" s="14"/>
+      <c r="DO8" s="14"/>
+      <c r="DP8" s="14"/>
+      <c r="DQ8" s="14"/>
+      <c r="DR8" s="14"/>
+      <c r="DS8" s="14"/>
+      <c r="DT8" s="14"/>
+      <c r="DU8" s="14"/>
+      <c r="DV8" s="14"/>
+      <c r="DW8" s="14"/>
+      <c r="DX8" s="14"/>
+      <c r="DY8" s="14"/>
+      <c r="DZ8" s="14"/>
+      <c r="EA8" s="14"/>
+      <c r="EB8" s="14"/>
+      <c r="EC8" s="14"/>
+      <c r="ED8" s="14"/>
+      <c r="EE8" s="14"/>
+      <c r="EF8" s="14"/>
+      <c r="EG8" s="14"/>
+      <c r="EH8" s="14"/>
+      <c r="EI8" s="14"/>
+      <c r="EJ8" s="14"/>
+      <c r="EK8" s="14"/>
+      <c r="EL8" s="14"/>
+      <c r="EM8" s="14"/>
+      <c r="EN8" s="14"/>
+      <c r="EO8" s="14"/>
+      <c r="EP8" s="14"/>
+      <c r="EQ8" s="14"/>
+      <c r="ER8" s="14"/>
+      <c r="ES8" s="14"/>
+      <c r="ET8" s="14"/>
+      <c r="EU8" s="14"/>
+      <c r="EV8" s="14"/>
+      <c r="EW8" s="14"/>
+      <c r="EX8" s="14"/>
+      <c r="EY8" s="14"/>
+      <c r="EZ8" s="14"/>
+      <c r="FA8" s="14"/>
+      <c r="FB8" s="14"/>
+      <c r="FC8" s="14"/>
+      <c r="FD8" s="14"/>
+      <c r="FE8" s="14"/>
+      <c r="FF8" s="14"/>
+      <c r="FG8" s="14"/>
+      <c r="FH8" s="14"/>
+      <c r="FI8" s="14"/>
+      <c r="FJ8" s="14"/>
+      <c r="FK8" s="14"/>
+      <c r="FL8" s="14"/>
+      <c r="FM8" s="14"/>
+      <c r="FN8" s="14"/>
+      <c r="FO8" s="14"/>
+      <c r="FP8" s="14"/>
+      <c r="FQ8" s="14"/>
+      <c r="FR8" s="14"/>
+      <c r="FS8" s="14"/>
+      <c r="FT8" s="14"/>
+      <c r="FU8" s="14"/>
+      <c r="FV8" s="14"/>
+      <c r="FW8" s="14"/>
+      <c r="FX8" s="14"/>
+      <c r="FY8" s="14"/>
+      <c r="FZ8" s="14"/>
+      <c r="GA8" s="14"/>
+      <c r="GB8" s="14"/>
+      <c r="GC8" s="14"/>
+      <c r="GD8" s="14"/>
+      <c r="GE8" s="14"/>
+      <c r="GF8" s="14"/>
+      <c r="GG8" s="14"/>
+      <c r="GH8" s="14"/>
+      <c r="GI8" s="14"/>
+      <c r="GJ8" s="14"/>
+      <c r="GK8" s="14"/>
+      <c r="GL8" s="14"/>
+      <c r="GM8" s="14"/>
+      <c r="GN8" s="14"/>
+      <c r="GO8" s="14"/>
+      <c r="GP8" s="14"/>
+      <c r="GQ8" s="14"/>
+      <c r="GR8" s="14"/>
+      <c r="GS8" s="14"/>
+      <c r="GT8" s="14"/>
+      <c r="GU8" s="14"/>
+      <c r="GV8" s="14"/>
+      <c r="GW8" s="14"/>
+      <c r="GX8" s="14"/>
+      <c r="GY8" s="14"/>
+      <c r="GZ8" s="14"/>
+      <c r="HA8" s="14"/>
+      <c r="HB8" s="14"/>
+      <c r="HC8" s="14"/>
+      <c r="HD8" s="14"/>
+      <c r="HE8" s="14"/>
+      <c r="HF8" s="14"/>
+      <c r="HG8" s="14"/>
+      <c r="HH8" s="14"/>
+      <c r="HI8" s="14"/>
+      <c r="HJ8" s="14"/>
+      <c r="HK8" s="14"/>
+      <c r="HL8" s="14"/>
+      <c r="HM8" s="14"/>
+      <c r="HN8" s="14"/>
+      <c r="HO8" s="14"/>
+      <c r="HP8" s="14"/>
+      <c r="HQ8" s="14"/>
+      <c r="HR8" s="14"/>
+      <c r="HS8" s="14"/>
+      <c r="HT8" s="14"/>
+      <c r="HU8" s="14"/>
+      <c r="HV8" s="14"/>
+      <c r="HW8" s="14"/>
+      <c r="HX8" s="14"/>
+      <c r="HY8" s="14"/>
+      <c r="HZ8" s="14"/>
+      <c r="IA8" s="14"/>
+      <c r="IB8" s="14"/>
+      <c r="IC8" s="14"/>
+      <c r="ID8" s="14"/>
+      <c r="IE8" s="14"/>
+      <c r="IF8" s="14"/>
+      <c r="IG8" s="14"/>
+      <c r="IH8" s="14"/>
+      <c r="II8" s="14"/>
+      <c r="IJ8" s="14"/>
+      <c r="IK8" s="14"/>
+      <c r="IL8" s="14"/>
+      <c r="IM8" s="14"/>
+      <c r="IN8" s="14"/>
+      <c r="IO8" s="14"/>
+      <c r="IP8" s="14"/>
+      <c r="IQ8" s="14"/>
+      <c r="IR8" s="14"/>
+      <c r="IS8" s="14"/>
+      <c r="IT8" s="14"/>
+      <c r="IU8" s="14"/>
+      <c r="IV8" s="14"/>
+      <c r="IW8" s="14"/>
+    </row>
+    <row r="9" s="18" customFormat="true" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>352</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>353</v>
-      </c>
-      <c r="G9" s="20" t="s">
+      <c r="E9" s="22" t="s">
         <v>354</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="F9" s="22" t="s">
         <v>355</v>
       </c>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="14"/>
-      <c r="AC9" s="14"/>
-      <c r="AD9" s="14"/>
-      <c r="AE9" s="14"/>
-      <c r="AF9" s="14"/>
-      <c r="AG9" s="14"/>
-      <c r="AH9" s="14"/>
-      <c r="AI9" s="14"/>
-      <c r="AJ9" s="14"/>
-      <c r="AK9" s="14"/>
-      <c r="AL9" s="14"/>
-      <c r="AM9" s="14"/>
-      <c r="AN9" s="14"/>
-      <c r="AO9" s="14"/>
-      <c r="AP9" s="14"/>
-      <c r="AQ9" s="14"/>
-      <c r="AR9" s="14"/>
-      <c r="AS9" s="14"/>
-      <c r="AT9" s="14"/>
-      <c r="AU9" s="14"/>
-      <c r="AV9" s="14"/>
-      <c r="AW9" s="14"/>
-      <c r="AX9" s="14"/>
-      <c r="AY9" s="14"/>
-      <c r="AZ9" s="14"/>
-      <c r="BA9" s="14"/>
-      <c r="BB9" s="14"/>
-      <c r="BC9" s="14"/>
-      <c r="BD9" s="14"/>
-      <c r="BE9" s="14"/>
-      <c r="BF9" s="14"/>
-      <c r="BG9" s="14"/>
-      <c r="BH9" s="14"/>
-      <c r="BI9" s="14"/>
-      <c r="BJ9" s="14"/>
-      <c r="BK9" s="14"/>
-      <c r="BL9" s="14"/>
-      <c r="BM9" s="14"/>
-      <c r="BN9" s="14"/>
-      <c r="BO9" s="14"/>
-      <c r="BP9" s="14"/>
-      <c r="BQ9" s="14"/>
-      <c r="BR9" s="14"/>
-      <c r="BS9" s="14"/>
-      <c r="BT9" s="14"/>
-      <c r="BU9" s="14"/>
-      <c r="BV9" s="14"/>
-      <c r="BW9" s="14"/>
-      <c r="BX9" s="14"/>
-      <c r="BY9" s="14"/>
-      <c r="BZ9" s="14"/>
-      <c r="CA9" s="14"/>
-      <c r="CB9" s="14"/>
-      <c r="CC9" s="14"/>
-      <c r="CD9" s="14"/>
-      <c r="CE9" s="14"/>
-      <c r="CF9" s="14"/>
-      <c r="CG9" s="14"/>
-      <c r="CH9" s="14"/>
-      <c r="CI9" s="14"/>
-      <c r="CJ9" s="14"/>
-      <c r="CK9" s="14"/>
-      <c r="CL9" s="14"/>
-      <c r="CM9" s="14"/>
-      <c r="CN9" s="14"/>
-      <c r="CO9" s="14"/>
-      <c r="CP9" s="14"/>
-      <c r="CQ9" s="14"/>
-      <c r="CR9" s="14"/>
-      <c r="CS9" s="14"/>
-      <c r="CT9" s="14"/>
-      <c r="CU9" s="14"/>
-      <c r="CV9" s="14"/>
-      <c r="CW9" s="14"/>
-      <c r="CX9" s="14"/>
-      <c r="CY9" s="14"/>
-      <c r="CZ9" s="14"/>
-      <c r="DA9" s="14"/>
-      <c r="DB9" s="14"/>
-      <c r="DC9" s="14"/>
-      <c r="DD9" s="14"/>
-      <c r="DE9" s="14"/>
-      <c r="DF9" s="14"/>
-      <c r="DG9" s="14"/>
-      <c r="DH9" s="14"/>
-      <c r="DI9" s="14"/>
-      <c r="DJ9" s="14"/>
-      <c r="DK9" s="14"/>
-      <c r="DL9" s="14"/>
-      <c r="DM9" s="14"/>
-      <c r="DN9" s="14"/>
-      <c r="DO9" s="14"/>
-      <c r="DP9" s="14"/>
-      <c r="DQ9" s="14"/>
-      <c r="DR9" s="14"/>
-      <c r="DS9" s="14"/>
-      <c r="DT9" s="14"/>
-      <c r="DU9" s="14"/>
-      <c r="DV9" s="14"/>
-      <c r="DW9" s="14"/>
-      <c r="DX9" s="14"/>
-      <c r="DY9" s="14"/>
-      <c r="DZ9" s="14"/>
-      <c r="EA9" s="14"/>
-      <c r="EB9" s="14"/>
-      <c r="EC9" s="14"/>
-      <c r="ED9" s="14"/>
-      <c r="EE9" s="14"/>
-      <c r="EF9" s="14"/>
-      <c r="EG9" s="14"/>
-      <c r="EH9" s="14"/>
-      <c r="EI9" s="14"/>
-      <c r="EJ9" s="14"/>
-      <c r="EK9" s="14"/>
-      <c r="EL9" s="14"/>
-      <c r="EM9" s="14"/>
-      <c r="EN9" s="14"/>
-      <c r="EO9" s="14"/>
-      <c r="EP9" s="14"/>
-      <c r="EQ9" s="14"/>
-      <c r="ER9" s="14"/>
-      <c r="ES9" s="14"/>
-      <c r="ET9" s="14"/>
-      <c r="EU9" s="14"/>
-      <c r="EV9" s="14"/>
-      <c r="EW9" s="14"/>
-      <c r="EX9" s="14"/>
-      <c r="EY9" s="14"/>
-      <c r="EZ9" s="14"/>
-      <c r="FA9" s="14"/>
-      <c r="FB9" s="14"/>
-      <c r="FC9" s="14"/>
-      <c r="FD9" s="14"/>
-      <c r="FE9" s="14"/>
-      <c r="FF9" s="14"/>
-      <c r="FG9" s="14"/>
-      <c r="FH9" s="14"/>
-      <c r="FI9" s="14"/>
-      <c r="FJ9" s="14"/>
-      <c r="FK9" s="14"/>
-      <c r="FL9" s="14"/>
-      <c r="FM9" s="14"/>
-      <c r="FN9" s="14"/>
-      <c r="FO9" s="14"/>
-      <c r="FP9" s="14"/>
-      <c r="FQ9" s="14"/>
-      <c r="FR9" s="14"/>
-      <c r="FS9" s="14"/>
-      <c r="FT9" s="14"/>
-      <c r="FU9" s="14"/>
-      <c r="FV9" s="14"/>
-      <c r="FW9" s="14"/>
-      <c r="FX9" s="14"/>
-      <c r="FY9" s="14"/>
-      <c r="FZ9" s="14"/>
-      <c r="GA9" s="14"/>
-      <c r="GB9" s="14"/>
-      <c r="GC9" s="14"/>
-      <c r="GD9" s="14"/>
-      <c r="GE9" s="14"/>
-      <c r="GF9" s="14"/>
-      <c r="GG9" s="14"/>
-      <c r="GH9" s="14"/>
-      <c r="GI9" s="14"/>
-      <c r="GJ9" s="14"/>
-      <c r="GK9" s="14"/>
-      <c r="GL9" s="14"/>
-      <c r="GM9" s="14"/>
-      <c r="GN9" s="14"/>
-      <c r="GO9" s="14"/>
-      <c r="GP9" s="14"/>
-      <c r="GQ9" s="14"/>
-      <c r="GR9" s="14"/>
-      <c r="GS9" s="14"/>
-      <c r="GT9" s="14"/>
-      <c r="GU9" s="14"/>
-      <c r="GV9" s="14"/>
-      <c r="GW9" s="14"/>
-      <c r="GX9" s="14"/>
-      <c r="GY9" s="14"/>
-      <c r="GZ9" s="14"/>
-      <c r="HA9" s="14"/>
-      <c r="HB9" s="14"/>
-      <c r="HC9" s="14"/>
-      <c r="HD9" s="14"/>
-      <c r="HE9" s="14"/>
-      <c r="HF9" s="14"/>
-      <c r="HG9" s="14"/>
-      <c r="HH9" s="14"/>
-      <c r="HI9" s="14"/>
-      <c r="HJ9" s="14"/>
-      <c r="HK9" s="14"/>
-      <c r="HL9" s="14"/>
-      <c r="HM9" s="14"/>
-      <c r="HN9" s="14"/>
-      <c r="HO9" s="14"/>
-      <c r="HP9" s="14"/>
-      <c r="HQ9" s="14"/>
-      <c r="HR9" s="14"/>
-      <c r="HS9" s="14"/>
-      <c r="HT9" s="14"/>
-      <c r="HU9" s="14"/>
-      <c r="HV9" s="14"/>
-      <c r="HW9" s="14"/>
-      <c r="HX9" s="14"/>
-      <c r="HY9" s="14"/>
-      <c r="HZ9" s="14"/>
-      <c r="IA9" s="14"/>
-      <c r="IB9" s="14"/>
-      <c r="IC9" s="14"/>
-      <c r="ID9" s="14"/>
-      <c r="IE9" s="14"/>
-      <c r="IF9" s="14"/>
-      <c r="IG9" s="14"/>
-      <c r="IH9" s="14"/>
-      <c r="II9" s="14"/>
-      <c r="IJ9" s="14"/>
-      <c r="IK9" s="14"/>
-      <c r="IL9" s="14"/>
-      <c r="IM9" s="14"/>
-      <c r="IN9" s="14"/>
-      <c r="IO9" s="14"/>
-      <c r="IP9" s="14"/>
-      <c r="IQ9" s="14"/>
-      <c r="IR9" s="14"/>
-      <c r="IS9" s="14"/>
-      <c r="IT9" s="14"/>
-      <c r="IU9" s="14"/>
-      <c r="IV9" s="14"/>
-      <c r="IW9" s="14"/>
+      <c r="G9" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="16"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9" s="16"/>
+      <c r="AF9" s="16"/>
+      <c r="AG9" s="16"/>
+      <c r="AH9" s="16"/>
+      <c r="AI9" s="16"/>
+      <c r="AJ9" s="16"/>
+      <c r="AK9" s="16"/>
+      <c r="AL9" s="16"/>
+      <c r="AM9" s="16"/>
+      <c r="AN9" s="16"/>
+      <c r="AO9" s="16"/>
+      <c r="AP9" s="16"/>
+      <c r="AQ9" s="16"/>
+      <c r="AR9" s="16"/>
+      <c r="AS9" s="16"/>
+      <c r="AT9" s="16"/>
+      <c r="AU9" s="16"/>
+      <c r="AV9" s="16"/>
+      <c r="AW9" s="16"/>
+      <c r="AX9" s="16"/>
+      <c r="AY9" s="16"/>
+      <c r="AZ9" s="16"/>
+      <c r="BA9" s="16"/>
+      <c r="BB9" s="16"/>
+      <c r="BC9" s="16"/>
+      <c r="BD9" s="16"/>
+      <c r="BE9" s="16"/>
+      <c r="BF9" s="16"/>
+      <c r="BG9" s="16"/>
+      <c r="BH9" s="16"/>
+      <c r="BI9" s="16"/>
+      <c r="BJ9" s="16"/>
+      <c r="BK9" s="16"/>
+      <c r="BL9" s="16"/>
+      <c r="BM9" s="16"/>
+      <c r="BN9" s="16"/>
+      <c r="BO9" s="16"/>
+      <c r="BP9" s="16"/>
+      <c r="BQ9" s="16"/>
+      <c r="BR9" s="16"/>
+      <c r="BS9" s="16"/>
+      <c r="BT9" s="16"/>
+      <c r="BU9" s="16"/>
+      <c r="BV9" s="16"/>
+      <c r="BW9" s="16"/>
+      <c r="BX9" s="16"/>
+      <c r="BY9" s="16"/>
+      <c r="BZ9" s="16"/>
+      <c r="CA9" s="16"/>
+      <c r="CB9" s="16"/>
+      <c r="CC9" s="16"/>
+      <c r="CD9" s="16"/>
+      <c r="CE9" s="16"/>
+      <c r="CF9" s="16"/>
+      <c r="CG9" s="16"/>
+      <c r="CH9" s="16"/>
+      <c r="CI9" s="16"/>
+      <c r="CJ9" s="16"/>
+      <c r="CK9" s="16"/>
+      <c r="CL9" s="16"/>
+      <c r="CM9" s="16"/>
+      <c r="CN9" s="16"/>
+      <c r="CO9" s="16"/>
+      <c r="CP9" s="16"/>
+      <c r="CQ9" s="16"/>
+      <c r="CR9" s="16"/>
+      <c r="CS9" s="16"/>
+      <c r="CT9" s="16"/>
+      <c r="CU9" s="16"/>
+      <c r="CV9" s="16"/>
+      <c r="CW9" s="16"/>
+      <c r="CX9" s="16"/>
+      <c r="CY9" s="16"/>
+      <c r="CZ9" s="16"/>
+      <c r="DA9" s="16"/>
+      <c r="DB9" s="16"/>
+      <c r="DC9" s="16"/>
+      <c r="DD9" s="16"/>
+      <c r="DE9" s="16"/>
+      <c r="DF9" s="16"/>
+      <c r="DG9" s="16"/>
+      <c r="DH9" s="16"/>
+      <c r="DI9" s="16"/>
+      <c r="DJ9" s="16"/>
+      <c r="DK9" s="16"/>
+      <c r="DL9" s="16"/>
+      <c r="DM9" s="16"/>
+      <c r="DN9" s="16"/>
+      <c r="DO9" s="16"/>
+      <c r="DP9" s="16"/>
+      <c r="DQ9" s="16"/>
+      <c r="DR9" s="16"/>
+      <c r="DS9" s="16"/>
+      <c r="DT9" s="16"/>
+      <c r="DU9" s="16"/>
+      <c r="DV9" s="16"/>
+      <c r="DW9" s="16"/>
+      <c r="DX9" s="16"/>
+      <c r="DY9" s="16"/>
+      <c r="DZ9" s="16"/>
+      <c r="EA9" s="16"/>
+      <c r="EB9" s="16"/>
+      <c r="EC9" s="16"/>
+      <c r="ED9" s="16"/>
+      <c r="EE9" s="16"/>
+      <c r="EF9" s="16"/>
+      <c r="EG9" s="16"/>
+      <c r="EH9" s="16"/>
+      <c r="EI9" s="16"/>
+      <c r="EJ9" s="16"/>
+      <c r="EK9" s="16"/>
+      <c r="EL9" s="16"/>
+      <c r="EM9" s="16"/>
+      <c r="EN9" s="16"/>
+      <c r="EO9" s="16"/>
+      <c r="EP9" s="16"/>
+      <c r="EQ9" s="16"/>
+      <c r="ER9" s="16"/>
+      <c r="ES9" s="16"/>
+      <c r="ET9" s="16"/>
+      <c r="EU9" s="16"/>
+      <c r="EV9" s="16"/>
+      <c r="EW9" s="16"/>
+      <c r="EX9" s="16"/>
+      <c r="EY9" s="16"/>
+      <c r="EZ9" s="16"/>
+      <c r="FA9" s="16"/>
+      <c r="FB9" s="16"/>
+      <c r="FC9" s="16"/>
+      <c r="FD9" s="16"/>
+      <c r="FE9" s="16"/>
+      <c r="FF9" s="16"/>
+      <c r="FG9" s="16"/>
+      <c r="FH9" s="16"/>
+      <c r="FI9" s="16"/>
+      <c r="FJ9" s="16"/>
+      <c r="FK9" s="16"/>
+      <c r="FL9" s="16"/>
+      <c r="FM9" s="16"/>
+      <c r="FN9" s="16"/>
+      <c r="FO9" s="16"/>
+      <c r="FP9" s="16"/>
+      <c r="FQ9" s="16"/>
+      <c r="FR9" s="16"/>
+      <c r="FS9" s="16"/>
+      <c r="FT9" s="16"/>
+      <c r="FU9" s="16"/>
+      <c r="FV9" s="16"/>
+      <c r="FW9" s="16"/>
+      <c r="FX9" s="16"/>
+      <c r="FY9" s="16"/>
+      <c r="FZ9" s="16"/>
+      <c r="GA9" s="16"/>
+      <c r="GB9" s="16"/>
+      <c r="GC9" s="16"/>
+      <c r="GD9" s="16"/>
+      <c r="GE9" s="16"/>
+      <c r="GF9" s="16"/>
+      <c r="GG9" s="16"/>
+      <c r="GH9" s="16"/>
+      <c r="GI9" s="16"/>
+      <c r="GJ9" s="16"/>
+      <c r="GK9" s="16"/>
+      <c r="GL9" s="16"/>
+      <c r="GM9" s="16"/>
+      <c r="GN9" s="16"/>
+      <c r="GO9" s="16"/>
+      <c r="GP9" s="16"/>
+      <c r="GQ9" s="16"/>
+      <c r="GR9" s="16"/>
+      <c r="GS9" s="16"/>
+      <c r="GT9" s="16"/>
+      <c r="GU9" s="16"/>
+      <c r="GV9" s="16"/>
+      <c r="GW9" s="16"/>
+      <c r="GX9" s="16"/>
+      <c r="GY9" s="16"/>
+      <c r="GZ9" s="16"/>
+      <c r="HA9" s="16"/>
+      <c r="HB9" s="16"/>
+      <c r="HC9" s="16"/>
+      <c r="HD9" s="16"/>
+      <c r="HE9" s="16"/>
+      <c r="HF9" s="16"/>
+      <c r="HG9" s="16"/>
+      <c r="HH9" s="16"/>
+      <c r="HI9" s="16"/>
+      <c r="HJ9" s="16"/>
+      <c r="HK9" s="16"/>
+      <c r="HL9" s="16"/>
+      <c r="HM9" s="16"/>
+      <c r="HN9" s="16"/>
+      <c r="HO9" s="16"/>
+      <c r="HP9" s="16"/>
+      <c r="HQ9" s="16"/>
+      <c r="HR9" s="16"/>
+      <c r="HS9" s="16"/>
+      <c r="HT9" s="16"/>
+      <c r="HU9" s="16"/>
+      <c r="HV9" s="16"/>
+      <c r="HW9" s="16"/>
+      <c r="HX9" s="16"/>
+      <c r="HY9" s="16"/>
+      <c r="HZ9" s="16"/>
+      <c r="IA9" s="16"/>
+      <c r="IB9" s="16"/>
+      <c r="IC9" s="16"/>
+      <c r="ID9" s="16"/>
+      <c r="IE9" s="16"/>
+      <c r="IF9" s="16"/>
+      <c r="IG9" s="16"/>
+      <c r="IH9" s="16"/>
+      <c r="II9" s="16"/>
+      <c r="IJ9" s="16"/>
+      <c r="IK9" s="16"/>
+      <c r="IL9" s="16"/>
+      <c r="IM9" s="16"/>
+      <c r="IN9" s="16"/>
+      <c r="IO9" s="16"/>
+      <c r="IP9" s="16"/>
+      <c r="IQ9" s="16"/>
+      <c r="IR9" s="16"/>
+      <c r="IS9" s="16"/>
+      <c r="IT9" s="16"/>
+      <c r="IU9" s="16"/>
+      <c r="IV9" s="16"/>
+      <c r="IW9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>347</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="A10" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="22" t="s">
-        <v>357</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>358</v>
-      </c>
-      <c r="G10" s="23" t="n">
+      <c r="E10" s="24" t="s">
+        <v>359</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="G10" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="H10" s="24" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="H10" s="26" t="s">
+        <v>361</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -5825,28 +6096,27 @@
       <c r="IW10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="25" t="s">
-        <v>359</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>347</v>
-      </c>
-      <c r="C11" s="17" t="s">
+      <c r="A11" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>361</v>
-      </c>
-      <c r="G11" s="23" t="n">
+      <c r="E11" s="24" t="s">
+        <v>363</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>364</v>
+      </c>
+      <c r="G11" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="27" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="H11" s="29" t="s">
+        <v>365</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -5858,26 +6128,25 @@
     </row>
     <row r="12" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>348</v>
-      </c>
-      <c r="C12" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="22" t="s">
-        <v>362</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="G12" s="23" t="n">
+      <c r="E12" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="G12" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="H12" s="28" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H12" s="30" t="b">
         <v>0</v>
       </c>
       <c r="I12" s="5"/>
@@ -5889,28 +6158,27 @@
       <c r="IW12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
-        <v>364</v>
-      </c>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="G13" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="26" t="s">
         <v>365</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="22" t="s">
-        <v>366</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>367</v>
-      </c>
-      <c r="G13" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="H13" s="24" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -5921,28 +6189,27 @@
       <c r="IW13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25" t="s">
-        <v>368</v>
-      </c>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="24" t="s">
+        <v>372</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="G14" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="H14" s="26" t="s">
         <v>365</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="22" t="s">
-        <v>369</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>370</v>
-      </c>
-      <c r="G14" s="23" t="n">
-        <v>4</v>
-      </c>
-      <c r="H14" s="24" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -5957,561 +6224,554 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="I15" s="29"/>
+      <c r="I15" s="31"/>
       <c r="IT15" s="4"/>
       <c r="IU15" s="4"/>
       <c r="IV15" s="4"/>
       <c r="IW15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31"/>
-    </row>
-    <row r="17" s="13" customFormat="true" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="s">
-        <v>371</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
-      <c r="AB17" s="12"/>
-      <c r="AC17" s="12"/>
-      <c r="AD17" s="12"/>
-      <c r="AE17" s="12"/>
-      <c r="AF17" s="12"/>
-      <c r="AG17" s="12"/>
-      <c r="AH17" s="12"/>
-      <c r="AI17" s="12"/>
-      <c r="AJ17" s="12"/>
-      <c r="AK17" s="12"/>
-      <c r="AL17" s="12"/>
-      <c r="AM17" s="12"/>
-      <c r="AN17" s="12"/>
-      <c r="AO17" s="12"/>
-      <c r="AP17" s="12"/>
-      <c r="AQ17" s="12"/>
-      <c r="AR17" s="12"/>
-      <c r="AS17" s="12"/>
-      <c r="AT17" s="12"/>
-      <c r="AU17" s="12"/>
-      <c r="AV17" s="12"/>
-      <c r="AW17" s="12"/>
-      <c r="AX17" s="12"/>
-      <c r="AY17" s="12"/>
-      <c r="AZ17" s="12"/>
-      <c r="BA17" s="12"/>
-      <c r="BB17" s="12"/>
-      <c r="BC17" s="12"/>
-      <c r="BD17" s="12"/>
-      <c r="BE17" s="12"/>
-      <c r="BF17" s="12"/>
-      <c r="BG17" s="12"/>
-      <c r="BH17" s="12"/>
-      <c r="BI17" s="12"/>
-      <c r="BJ17" s="12"/>
-      <c r="BK17" s="12"/>
-      <c r="BL17" s="12"/>
-      <c r="BM17" s="12"/>
-      <c r="BN17" s="12"/>
-      <c r="BO17" s="12"/>
-      <c r="BP17" s="12"/>
-      <c r="BQ17" s="12"/>
-      <c r="BR17" s="12"/>
-      <c r="BS17" s="12"/>
-      <c r="BT17" s="12"/>
-      <c r="BU17" s="12"/>
-      <c r="BV17" s="12"/>
-      <c r="BW17" s="12"/>
-      <c r="BX17" s="12"/>
-      <c r="BY17" s="12"/>
-      <c r="BZ17" s="12"/>
-      <c r="CA17" s="12"/>
-      <c r="CB17" s="12"/>
-      <c r="CC17" s="12"/>
-      <c r="CD17" s="12"/>
-      <c r="CE17" s="12"/>
-      <c r="CF17" s="12"/>
-      <c r="CG17" s="12"/>
-      <c r="CH17" s="12"/>
-      <c r="CI17" s="12"/>
-      <c r="CJ17" s="12"/>
-      <c r="CK17" s="12"/>
-      <c r="CL17" s="12"/>
-      <c r="CM17" s="12"/>
-      <c r="CN17" s="12"/>
-      <c r="CO17" s="12"/>
-      <c r="CP17" s="12"/>
-      <c r="CQ17" s="12"/>
-      <c r="CR17" s="12"/>
-      <c r="CS17" s="12"/>
-      <c r="CT17" s="12"/>
-      <c r="CU17" s="12"/>
-      <c r="CV17" s="12"/>
-      <c r="CW17" s="12"/>
-      <c r="CX17" s="12"/>
-      <c r="CY17" s="12"/>
-      <c r="CZ17" s="12"/>
-      <c r="DA17" s="12"/>
-      <c r="DB17" s="12"/>
-      <c r="DC17" s="12"/>
-      <c r="DD17" s="12"/>
-      <c r="DE17" s="12"/>
-      <c r="DF17" s="12"/>
-      <c r="DG17" s="12"/>
-      <c r="DH17" s="12"/>
-      <c r="DI17" s="12"/>
-      <c r="DJ17" s="12"/>
-      <c r="DK17" s="12"/>
-      <c r="DL17" s="12"/>
-      <c r="DM17" s="12"/>
-      <c r="DN17" s="12"/>
-      <c r="DO17" s="12"/>
-      <c r="DP17" s="12"/>
-      <c r="DQ17" s="12"/>
-      <c r="DR17" s="12"/>
-      <c r="DS17" s="12"/>
-      <c r="DT17" s="12"/>
-      <c r="DU17" s="12"/>
-      <c r="DV17" s="12"/>
-      <c r="DW17" s="12"/>
-      <c r="DX17" s="12"/>
-      <c r="DY17" s="12"/>
-      <c r="DZ17" s="12"/>
-      <c r="EA17" s="12"/>
-      <c r="EB17" s="12"/>
-      <c r="EC17" s="12"/>
-      <c r="ED17" s="12"/>
-      <c r="EE17" s="12"/>
-      <c r="EF17" s="12"/>
-      <c r="EG17" s="12"/>
-      <c r="EH17" s="12"/>
-      <c r="EI17" s="12"/>
-      <c r="EJ17" s="12"/>
-      <c r="EK17" s="12"/>
-      <c r="EL17" s="12"/>
-      <c r="EM17" s="12"/>
-      <c r="EN17" s="12"/>
-      <c r="EO17" s="12"/>
-      <c r="EP17" s="12"/>
-      <c r="EQ17" s="12"/>
-      <c r="ER17" s="12"/>
-      <c r="ES17" s="12"/>
-      <c r="ET17" s="12"/>
-      <c r="EU17" s="12"/>
-      <c r="EV17" s="12"/>
-      <c r="EW17" s="12"/>
-      <c r="EX17" s="12"/>
-      <c r="EY17" s="12"/>
-      <c r="EZ17" s="12"/>
-      <c r="FA17" s="12"/>
-      <c r="FB17" s="12"/>
-      <c r="FC17" s="12"/>
-      <c r="FD17" s="12"/>
-      <c r="FE17" s="12"/>
-      <c r="FF17" s="12"/>
-      <c r="FG17" s="12"/>
-      <c r="FH17" s="12"/>
-      <c r="FI17" s="12"/>
-      <c r="FJ17" s="12"/>
-      <c r="FK17" s="12"/>
-      <c r="FL17" s="12"/>
-      <c r="FM17" s="12"/>
-      <c r="FN17" s="12"/>
-      <c r="FO17" s="12"/>
-      <c r="FP17" s="12"/>
-      <c r="FQ17" s="12"/>
-      <c r="FR17" s="12"/>
-      <c r="FS17" s="12"/>
-      <c r="FT17" s="12"/>
-      <c r="FU17" s="12"/>
-      <c r="FV17" s="12"/>
-      <c r="FW17" s="12"/>
-      <c r="FX17" s="12"/>
-      <c r="FY17" s="12"/>
-      <c r="FZ17" s="12"/>
-      <c r="GA17" s="12"/>
-      <c r="GB17" s="12"/>
-      <c r="GC17" s="12"/>
-      <c r="GD17" s="12"/>
-      <c r="GE17" s="12"/>
-      <c r="GF17" s="12"/>
-      <c r="GG17" s="12"/>
-      <c r="GH17" s="12"/>
-      <c r="GI17" s="12"/>
-      <c r="GJ17" s="12"/>
-      <c r="GK17" s="12"/>
-      <c r="GL17" s="12"/>
-      <c r="GM17" s="12"/>
-      <c r="GN17" s="12"/>
-      <c r="GO17" s="12"/>
-      <c r="GP17" s="12"/>
-      <c r="GQ17" s="12"/>
-      <c r="GR17" s="12"/>
-      <c r="GS17" s="12"/>
-      <c r="GT17" s="12"/>
-      <c r="GU17" s="12"/>
-      <c r="GV17" s="12"/>
-      <c r="GW17" s="12"/>
-      <c r="GX17" s="12"/>
-      <c r="GY17" s="12"/>
-      <c r="GZ17" s="12"/>
-      <c r="HA17" s="12"/>
-      <c r="HB17" s="12"/>
-      <c r="HC17" s="12"/>
-      <c r="HD17" s="12"/>
-      <c r="HE17" s="12"/>
-      <c r="HF17" s="12"/>
-      <c r="HG17" s="12"/>
-      <c r="HH17" s="12"/>
-      <c r="HI17" s="12"/>
-      <c r="HJ17" s="12"/>
-      <c r="HK17" s="12"/>
-      <c r="HL17" s="12"/>
-      <c r="HM17" s="12"/>
-      <c r="HN17" s="12"/>
-      <c r="HO17" s="12"/>
-      <c r="HP17" s="12"/>
-      <c r="HQ17" s="12"/>
-      <c r="HR17" s="12"/>
-      <c r="HS17" s="12"/>
-      <c r="HT17" s="12"/>
-      <c r="HU17" s="12"/>
-      <c r="HV17" s="12"/>
-      <c r="HW17" s="12"/>
-      <c r="HX17" s="12"/>
-      <c r="HY17" s="12"/>
-      <c r="HZ17" s="12"/>
-      <c r="IA17" s="12"/>
-      <c r="IB17" s="12"/>
-      <c r="IC17" s="12"/>
-      <c r="ID17" s="12"/>
-      <c r="IE17" s="12"/>
-      <c r="IF17" s="12"/>
-      <c r="IG17" s="12"/>
-      <c r="IH17" s="12"/>
-      <c r="II17" s="12"/>
-      <c r="IJ17" s="12"/>
-      <c r="IK17" s="12"/>
-      <c r="IL17" s="12"/>
-      <c r="IM17" s="12"/>
-      <c r="IN17" s="12"/>
-      <c r="IO17" s="12"/>
-      <c r="IP17" s="12"/>
-      <c r="IQ17" s="12"/>
-      <c r="IR17" s="12"/>
-      <c r="IS17" s="12"/>
-    </row>
-    <row r="18" s="16" customFormat="true" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="s">
-        <v>353</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="14"/>
-      <c r="Y18" s="14"/>
-      <c r="Z18" s="14"/>
-      <c r="AA18" s="14"/>
-      <c r="AB18" s="14"/>
-      <c r="AC18" s="14"/>
-      <c r="AD18" s="14"/>
-      <c r="AE18" s="14"/>
-      <c r="AF18" s="14"/>
-      <c r="AG18" s="14"/>
-      <c r="AH18" s="14"/>
-      <c r="AI18" s="14"/>
-      <c r="AJ18" s="14"/>
-      <c r="AK18" s="14"/>
-      <c r="AL18" s="14"/>
-      <c r="AM18" s="14"/>
-      <c r="AN18" s="14"/>
-      <c r="AO18" s="14"/>
-      <c r="AP18" s="14"/>
-      <c r="AQ18" s="14"/>
-      <c r="AR18" s="14"/>
-      <c r="AS18" s="14"/>
-      <c r="AT18" s="14"/>
-      <c r="AU18" s="14"/>
-      <c r="AV18" s="14"/>
-      <c r="AW18" s="14"/>
-      <c r="AX18" s="14"/>
-      <c r="AY18" s="14"/>
-      <c r="AZ18" s="14"/>
-      <c r="BA18" s="14"/>
-      <c r="BB18" s="14"/>
-      <c r="BC18" s="14"/>
-      <c r="BD18" s="14"/>
-      <c r="BE18" s="14"/>
-      <c r="BF18" s="14"/>
-      <c r="BG18" s="14"/>
-      <c r="BH18" s="14"/>
-      <c r="BI18" s="14"/>
-      <c r="BJ18" s="14"/>
-      <c r="BK18" s="14"/>
-      <c r="BL18" s="14"/>
-      <c r="BM18" s="14"/>
-      <c r="BN18" s="14"/>
-      <c r="BO18" s="14"/>
-      <c r="BP18" s="14"/>
-      <c r="BQ18" s="14"/>
-      <c r="BR18" s="14"/>
-      <c r="BS18" s="14"/>
-      <c r="BT18" s="14"/>
-      <c r="BU18" s="14"/>
-      <c r="BV18" s="14"/>
-      <c r="BW18" s="14"/>
-      <c r="BX18" s="14"/>
-      <c r="BY18" s="14"/>
-      <c r="BZ18" s="14"/>
-      <c r="CA18" s="14"/>
-      <c r="CB18" s="14"/>
-      <c r="CC18" s="14"/>
-      <c r="CD18" s="14"/>
-      <c r="CE18" s="14"/>
-      <c r="CF18" s="14"/>
-      <c r="CG18" s="14"/>
-      <c r="CH18" s="14"/>
-      <c r="CI18" s="14"/>
-      <c r="CJ18" s="14"/>
-      <c r="CK18" s="14"/>
-      <c r="CL18" s="14"/>
-      <c r="CM18" s="14"/>
-      <c r="CN18" s="14"/>
-      <c r="CO18" s="14"/>
-      <c r="CP18" s="14"/>
-      <c r="CQ18" s="14"/>
-      <c r="CR18" s="14"/>
-      <c r="CS18" s="14"/>
-      <c r="CT18" s="14"/>
-      <c r="CU18" s="14"/>
-      <c r="CV18" s="14"/>
-      <c r="CW18" s="14"/>
-      <c r="CX18" s="14"/>
-      <c r="CY18" s="14"/>
-      <c r="CZ18" s="14"/>
-      <c r="DA18" s="14"/>
-      <c r="DB18" s="14"/>
-      <c r="DC18" s="14"/>
-      <c r="DD18" s="14"/>
-      <c r="DE18" s="14"/>
-      <c r="DF18" s="14"/>
-      <c r="DG18" s="14"/>
-      <c r="DH18" s="14"/>
-      <c r="DI18" s="14"/>
-      <c r="DJ18" s="14"/>
-      <c r="DK18" s="14"/>
-      <c r="DL18" s="14"/>
-      <c r="DM18" s="14"/>
-      <c r="DN18" s="14"/>
-      <c r="DO18" s="14"/>
-      <c r="DP18" s="14"/>
-      <c r="DQ18" s="14"/>
-      <c r="DR18" s="14"/>
-      <c r="DS18" s="14"/>
-      <c r="DT18" s="14"/>
-      <c r="DU18" s="14"/>
-      <c r="DV18" s="14"/>
-      <c r="DW18" s="14"/>
-      <c r="DX18" s="14"/>
-      <c r="DY18" s="14"/>
-      <c r="DZ18" s="14"/>
-      <c r="EA18" s="14"/>
-      <c r="EB18" s="14"/>
-      <c r="EC18" s="14"/>
-      <c r="ED18" s="14"/>
-      <c r="EE18" s="14"/>
-      <c r="EF18" s="14"/>
-      <c r="EG18" s="14"/>
-      <c r="EH18" s="14"/>
-      <c r="EI18" s="14"/>
-      <c r="EJ18" s="14"/>
-      <c r="EK18" s="14"/>
-      <c r="EL18" s="14"/>
-      <c r="EM18" s="14"/>
-      <c r="EN18" s="14"/>
-      <c r="EO18" s="14"/>
-      <c r="EP18" s="14"/>
-      <c r="EQ18" s="14"/>
-      <c r="ER18" s="14"/>
-      <c r="ES18" s="14"/>
-      <c r="ET18" s="14"/>
-      <c r="EU18" s="14"/>
-      <c r="EV18" s="14"/>
-      <c r="EW18" s="14"/>
-      <c r="EX18" s="14"/>
-      <c r="EY18" s="14"/>
-      <c r="EZ18" s="14"/>
-      <c r="FA18" s="14"/>
-      <c r="FB18" s="14"/>
-      <c r="FC18" s="14"/>
-      <c r="FD18" s="14"/>
-      <c r="FE18" s="14"/>
-      <c r="FF18" s="14"/>
-      <c r="FG18" s="14"/>
-      <c r="FH18" s="14"/>
-      <c r="FI18" s="14"/>
-      <c r="FJ18" s="14"/>
-      <c r="FK18" s="14"/>
-      <c r="FL18" s="14"/>
-      <c r="FM18" s="14"/>
-      <c r="FN18" s="14"/>
-      <c r="FO18" s="14"/>
-      <c r="FP18" s="14"/>
-      <c r="FQ18" s="14"/>
-      <c r="FR18" s="14"/>
-      <c r="FS18" s="14"/>
-      <c r="FT18" s="14"/>
-      <c r="FU18" s="14"/>
-      <c r="FV18" s="14"/>
-      <c r="FW18" s="14"/>
-      <c r="FX18" s="14"/>
-      <c r="FY18" s="14"/>
-      <c r="FZ18" s="14"/>
-      <c r="GA18" s="14"/>
-      <c r="GB18" s="14"/>
-      <c r="GC18" s="14"/>
-      <c r="GD18" s="14"/>
-      <c r="GE18" s="14"/>
-      <c r="GF18" s="14"/>
-      <c r="GG18" s="14"/>
-      <c r="GH18" s="14"/>
-      <c r="GI18" s="14"/>
-      <c r="GJ18" s="14"/>
-      <c r="GK18" s="14"/>
-      <c r="GL18" s="14"/>
-      <c r="GM18" s="14"/>
-      <c r="GN18" s="14"/>
-      <c r="GO18" s="14"/>
-      <c r="GP18" s="14"/>
-      <c r="GQ18" s="14"/>
-      <c r="GR18" s="14"/>
-      <c r="GS18" s="14"/>
-      <c r="GT18" s="14"/>
-      <c r="GU18" s="14"/>
-      <c r="GV18" s="14"/>
-      <c r="GW18" s="14"/>
-      <c r="GX18" s="14"/>
-      <c r="GY18" s="14"/>
-      <c r="GZ18" s="14"/>
-      <c r="HA18" s="14"/>
-      <c r="HB18" s="14"/>
-      <c r="HC18" s="14"/>
-      <c r="HD18" s="14"/>
-      <c r="HE18" s="14"/>
-      <c r="HF18" s="14"/>
-      <c r="HG18" s="14"/>
-      <c r="HH18" s="14"/>
-      <c r="HI18" s="14"/>
-      <c r="HJ18" s="14"/>
-      <c r="HK18" s="14"/>
-      <c r="HL18" s="14"/>
-      <c r="HM18" s="14"/>
-      <c r="HN18" s="14"/>
-      <c r="HO18" s="14"/>
-      <c r="HP18" s="14"/>
-      <c r="HQ18" s="14"/>
-      <c r="HR18" s="14"/>
-      <c r="HS18" s="14"/>
-      <c r="HT18" s="14"/>
-      <c r="HU18" s="14"/>
-      <c r="HV18" s="14"/>
-      <c r="HW18" s="14"/>
-      <c r="HX18" s="14"/>
-      <c r="HY18" s="14"/>
-      <c r="HZ18" s="14"/>
-      <c r="IA18" s="14"/>
-      <c r="IB18" s="14"/>
-      <c r="IC18" s="14"/>
-      <c r="ID18" s="14"/>
-      <c r="IE18" s="14"/>
-      <c r="IF18" s="14"/>
-      <c r="IG18" s="14"/>
-      <c r="IH18" s="14"/>
-      <c r="II18" s="14"/>
-      <c r="IJ18" s="14"/>
-      <c r="IK18" s="14"/>
-      <c r="IL18" s="14"/>
-      <c r="IM18" s="14"/>
-      <c r="IN18" s="14"/>
-      <c r="IO18" s="14"/>
-      <c r="IP18" s="14"/>
-      <c r="IQ18" s="14"/>
-      <c r="IR18" s="14"/>
-      <c r="IS18" s="14"/>
+    <row r="16" s="15" customFormat="true" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="14"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="14"/>
+      <c r="AE16" s="14"/>
+      <c r="AF16" s="14"/>
+      <c r="AG16" s="14"/>
+      <c r="AH16" s="14"/>
+      <c r="AI16" s="14"/>
+      <c r="AJ16" s="14"/>
+      <c r="AK16" s="14"/>
+      <c r="AL16" s="14"/>
+      <c r="AM16" s="14"/>
+      <c r="AN16" s="14"/>
+      <c r="AO16" s="14"/>
+      <c r="AP16" s="14"/>
+      <c r="AQ16" s="14"/>
+      <c r="AR16" s="14"/>
+      <c r="AS16" s="14"/>
+      <c r="AT16" s="14"/>
+      <c r="AU16" s="14"/>
+      <c r="AV16" s="14"/>
+      <c r="AW16" s="14"/>
+      <c r="AX16" s="14"/>
+      <c r="AY16" s="14"/>
+      <c r="AZ16" s="14"/>
+      <c r="BA16" s="14"/>
+      <c r="BB16" s="14"/>
+      <c r="BC16" s="14"/>
+      <c r="BD16" s="14"/>
+      <c r="BE16" s="14"/>
+      <c r="BF16" s="14"/>
+      <c r="BG16" s="14"/>
+      <c r="BH16" s="14"/>
+      <c r="BI16" s="14"/>
+      <c r="BJ16" s="14"/>
+      <c r="BK16" s="14"/>
+      <c r="BL16" s="14"/>
+      <c r="BM16" s="14"/>
+      <c r="BN16" s="14"/>
+      <c r="BO16" s="14"/>
+      <c r="BP16" s="14"/>
+      <c r="BQ16" s="14"/>
+      <c r="BR16" s="14"/>
+      <c r="BS16" s="14"/>
+      <c r="BT16" s="14"/>
+      <c r="BU16" s="14"/>
+      <c r="BV16" s="14"/>
+      <c r="BW16" s="14"/>
+      <c r="BX16" s="14"/>
+      <c r="BY16" s="14"/>
+      <c r="BZ16" s="14"/>
+      <c r="CA16" s="14"/>
+      <c r="CB16" s="14"/>
+      <c r="CC16" s="14"/>
+      <c r="CD16" s="14"/>
+      <c r="CE16" s="14"/>
+      <c r="CF16" s="14"/>
+      <c r="CG16" s="14"/>
+      <c r="CH16" s="14"/>
+      <c r="CI16" s="14"/>
+      <c r="CJ16" s="14"/>
+      <c r="CK16" s="14"/>
+      <c r="CL16" s="14"/>
+      <c r="CM16" s="14"/>
+      <c r="CN16" s="14"/>
+      <c r="CO16" s="14"/>
+      <c r="CP16" s="14"/>
+      <c r="CQ16" s="14"/>
+      <c r="CR16" s="14"/>
+      <c r="CS16" s="14"/>
+      <c r="CT16" s="14"/>
+      <c r="CU16" s="14"/>
+      <c r="CV16" s="14"/>
+      <c r="CW16" s="14"/>
+      <c r="CX16" s="14"/>
+      <c r="CY16" s="14"/>
+      <c r="CZ16" s="14"/>
+      <c r="DA16" s="14"/>
+      <c r="DB16" s="14"/>
+      <c r="DC16" s="14"/>
+      <c r="DD16" s="14"/>
+      <c r="DE16" s="14"/>
+      <c r="DF16" s="14"/>
+      <c r="DG16" s="14"/>
+      <c r="DH16" s="14"/>
+      <c r="DI16" s="14"/>
+      <c r="DJ16" s="14"/>
+      <c r="DK16" s="14"/>
+      <c r="DL16" s="14"/>
+      <c r="DM16" s="14"/>
+      <c r="DN16" s="14"/>
+      <c r="DO16" s="14"/>
+      <c r="DP16" s="14"/>
+      <c r="DQ16" s="14"/>
+      <c r="DR16" s="14"/>
+      <c r="DS16" s="14"/>
+      <c r="DT16" s="14"/>
+      <c r="DU16" s="14"/>
+      <c r="DV16" s="14"/>
+      <c r="DW16" s="14"/>
+      <c r="DX16" s="14"/>
+      <c r="DY16" s="14"/>
+      <c r="DZ16" s="14"/>
+      <c r="EA16" s="14"/>
+      <c r="EB16" s="14"/>
+      <c r="EC16" s="14"/>
+      <c r="ED16" s="14"/>
+      <c r="EE16" s="14"/>
+      <c r="EF16" s="14"/>
+      <c r="EG16" s="14"/>
+      <c r="EH16" s="14"/>
+      <c r="EI16" s="14"/>
+      <c r="EJ16" s="14"/>
+      <c r="EK16" s="14"/>
+      <c r="EL16" s="14"/>
+      <c r="EM16" s="14"/>
+      <c r="EN16" s="14"/>
+      <c r="EO16" s="14"/>
+      <c r="EP16" s="14"/>
+      <c r="EQ16" s="14"/>
+      <c r="ER16" s="14"/>
+      <c r="ES16" s="14"/>
+      <c r="ET16" s="14"/>
+      <c r="EU16" s="14"/>
+      <c r="EV16" s="14"/>
+      <c r="EW16" s="14"/>
+      <c r="EX16" s="14"/>
+      <c r="EY16" s="14"/>
+      <c r="EZ16" s="14"/>
+      <c r="FA16" s="14"/>
+      <c r="FB16" s="14"/>
+      <c r="FC16" s="14"/>
+      <c r="FD16" s="14"/>
+      <c r="FE16" s="14"/>
+      <c r="FF16" s="14"/>
+      <c r="FG16" s="14"/>
+      <c r="FH16" s="14"/>
+      <c r="FI16" s="14"/>
+      <c r="FJ16" s="14"/>
+      <c r="FK16" s="14"/>
+      <c r="FL16" s="14"/>
+      <c r="FM16" s="14"/>
+      <c r="FN16" s="14"/>
+      <c r="FO16" s="14"/>
+      <c r="FP16" s="14"/>
+      <c r="FQ16" s="14"/>
+      <c r="FR16" s="14"/>
+      <c r="FS16" s="14"/>
+      <c r="FT16" s="14"/>
+      <c r="FU16" s="14"/>
+      <c r="FV16" s="14"/>
+      <c r="FW16" s="14"/>
+      <c r="FX16" s="14"/>
+      <c r="FY16" s="14"/>
+      <c r="FZ16" s="14"/>
+      <c r="GA16" s="14"/>
+      <c r="GB16" s="14"/>
+      <c r="GC16" s="14"/>
+      <c r="GD16" s="14"/>
+      <c r="GE16" s="14"/>
+      <c r="GF16" s="14"/>
+      <c r="GG16" s="14"/>
+      <c r="GH16" s="14"/>
+      <c r="GI16" s="14"/>
+      <c r="GJ16" s="14"/>
+      <c r="GK16" s="14"/>
+      <c r="GL16" s="14"/>
+      <c r="GM16" s="14"/>
+      <c r="GN16" s="14"/>
+      <c r="GO16" s="14"/>
+      <c r="GP16" s="14"/>
+      <c r="GQ16" s="14"/>
+      <c r="GR16" s="14"/>
+      <c r="GS16" s="14"/>
+      <c r="GT16" s="14"/>
+      <c r="GU16" s="14"/>
+      <c r="GV16" s="14"/>
+      <c r="GW16" s="14"/>
+      <c r="GX16" s="14"/>
+      <c r="GY16" s="14"/>
+      <c r="GZ16" s="14"/>
+      <c r="HA16" s="14"/>
+      <c r="HB16" s="14"/>
+      <c r="HC16" s="14"/>
+      <c r="HD16" s="14"/>
+      <c r="HE16" s="14"/>
+      <c r="HF16" s="14"/>
+      <c r="HG16" s="14"/>
+      <c r="HH16" s="14"/>
+      <c r="HI16" s="14"/>
+      <c r="HJ16" s="14"/>
+      <c r="HK16" s="14"/>
+      <c r="HL16" s="14"/>
+      <c r="HM16" s="14"/>
+      <c r="HN16" s="14"/>
+      <c r="HO16" s="14"/>
+      <c r="HP16" s="14"/>
+      <c r="HQ16" s="14"/>
+      <c r="HR16" s="14"/>
+      <c r="HS16" s="14"/>
+      <c r="HT16" s="14"/>
+      <c r="HU16" s="14"/>
+      <c r="HV16" s="14"/>
+      <c r="HW16" s="14"/>
+      <c r="HX16" s="14"/>
+      <c r="HY16" s="14"/>
+      <c r="HZ16" s="14"/>
+      <c r="IA16" s="14"/>
+      <c r="IB16" s="14"/>
+      <c r="IC16" s="14"/>
+      <c r="ID16" s="14"/>
+      <c r="IE16" s="14"/>
+      <c r="IF16" s="14"/>
+      <c r="IG16" s="14"/>
+      <c r="IH16" s="14"/>
+      <c r="II16" s="14"/>
+      <c r="IJ16" s="14"/>
+      <c r="IK16" s="14"/>
+      <c r="IL16" s="14"/>
+      <c r="IM16" s="14"/>
+      <c r="IN16" s="14"/>
+      <c r="IO16" s="14"/>
+      <c r="IP16" s="14"/>
+      <c r="IQ16" s="14"/>
+      <c r="IR16" s="14"/>
+      <c r="IS16" s="14"/>
+    </row>
+    <row r="17" s="18" customFormat="true" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>375</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="16"/>
+      <c r="Z17" s="16"/>
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="16"/>
+      <c r="AC17" s="16"/>
+      <c r="AD17" s="16"/>
+      <c r="AE17" s="16"/>
+      <c r="AF17" s="16"/>
+      <c r="AG17" s="16"/>
+      <c r="AH17" s="16"/>
+      <c r="AI17" s="16"/>
+      <c r="AJ17" s="16"/>
+      <c r="AK17" s="16"/>
+      <c r="AL17" s="16"/>
+      <c r="AM17" s="16"/>
+      <c r="AN17" s="16"/>
+      <c r="AO17" s="16"/>
+      <c r="AP17" s="16"/>
+      <c r="AQ17" s="16"/>
+      <c r="AR17" s="16"/>
+      <c r="AS17" s="16"/>
+      <c r="AT17" s="16"/>
+      <c r="AU17" s="16"/>
+      <c r="AV17" s="16"/>
+      <c r="AW17" s="16"/>
+      <c r="AX17" s="16"/>
+      <c r="AY17" s="16"/>
+      <c r="AZ17" s="16"/>
+      <c r="BA17" s="16"/>
+      <c r="BB17" s="16"/>
+      <c r="BC17" s="16"/>
+      <c r="BD17" s="16"/>
+      <c r="BE17" s="16"/>
+      <c r="BF17" s="16"/>
+      <c r="BG17" s="16"/>
+      <c r="BH17" s="16"/>
+      <c r="BI17" s="16"/>
+      <c r="BJ17" s="16"/>
+      <c r="BK17" s="16"/>
+      <c r="BL17" s="16"/>
+      <c r="BM17" s="16"/>
+      <c r="BN17" s="16"/>
+      <c r="BO17" s="16"/>
+      <c r="BP17" s="16"/>
+      <c r="BQ17" s="16"/>
+      <c r="BR17" s="16"/>
+      <c r="BS17" s="16"/>
+      <c r="BT17" s="16"/>
+      <c r="BU17" s="16"/>
+      <c r="BV17" s="16"/>
+      <c r="BW17" s="16"/>
+      <c r="BX17" s="16"/>
+      <c r="BY17" s="16"/>
+      <c r="BZ17" s="16"/>
+      <c r="CA17" s="16"/>
+      <c r="CB17" s="16"/>
+      <c r="CC17" s="16"/>
+      <c r="CD17" s="16"/>
+      <c r="CE17" s="16"/>
+      <c r="CF17" s="16"/>
+      <c r="CG17" s="16"/>
+      <c r="CH17" s="16"/>
+      <c r="CI17" s="16"/>
+      <c r="CJ17" s="16"/>
+      <c r="CK17" s="16"/>
+      <c r="CL17" s="16"/>
+      <c r="CM17" s="16"/>
+      <c r="CN17" s="16"/>
+      <c r="CO17" s="16"/>
+      <c r="CP17" s="16"/>
+      <c r="CQ17" s="16"/>
+      <c r="CR17" s="16"/>
+      <c r="CS17" s="16"/>
+      <c r="CT17" s="16"/>
+      <c r="CU17" s="16"/>
+      <c r="CV17" s="16"/>
+      <c r="CW17" s="16"/>
+      <c r="CX17" s="16"/>
+      <c r="CY17" s="16"/>
+      <c r="CZ17" s="16"/>
+      <c r="DA17" s="16"/>
+      <c r="DB17" s="16"/>
+      <c r="DC17" s="16"/>
+      <c r="DD17" s="16"/>
+      <c r="DE17" s="16"/>
+      <c r="DF17" s="16"/>
+      <c r="DG17" s="16"/>
+      <c r="DH17" s="16"/>
+      <c r="DI17" s="16"/>
+      <c r="DJ17" s="16"/>
+      <c r="DK17" s="16"/>
+      <c r="DL17" s="16"/>
+      <c r="DM17" s="16"/>
+      <c r="DN17" s="16"/>
+      <c r="DO17" s="16"/>
+      <c r="DP17" s="16"/>
+      <c r="DQ17" s="16"/>
+      <c r="DR17" s="16"/>
+      <c r="DS17" s="16"/>
+      <c r="DT17" s="16"/>
+      <c r="DU17" s="16"/>
+      <c r="DV17" s="16"/>
+      <c r="DW17" s="16"/>
+      <c r="DX17" s="16"/>
+      <c r="DY17" s="16"/>
+      <c r="DZ17" s="16"/>
+      <c r="EA17" s="16"/>
+      <c r="EB17" s="16"/>
+      <c r="EC17" s="16"/>
+      <c r="ED17" s="16"/>
+      <c r="EE17" s="16"/>
+      <c r="EF17" s="16"/>
+      <c r="EG17" s="16"/>
+      <c r="EH17" s="16"/>
+      <c r="EI17" s="16"/>
+      <c r="EJ17" s="16"/>
+      <c r="EK17" s="16"/>
+      <c r="EL17" s="16"/>
+      <c r="EM17" s="16"/>
+      <c r="EN17" s="16"/>
+      <c r="EO17" s="16"/>
+      <c r="EP17" s="16"/>
+      <c r="EQ17" s="16"/>
+      <c r="ER17" s="16"/>
+      <c r="ES17" s="16"/>
+      <c r="ET17" s="16"/>
+      <c r="EU17" s="16"/>
+      <c r="EV17" s="16"/>
+      <c r="EW17" s="16"/>
+      <c r="EX17" s="16"/>
+      <c r="EY17" s="16"/>
+      <c r="EZ17" s="16"/>
+      <c r="FA17" s="16"/>
+      <c r="FB17" s="16"/>
+      <c r="FC17" s="16"/>
+      <c r="FD17" s="16"/>
+      <c r="FE17" s="16"/>
+      <c r="FF17" s="16"/>
+      <c r="FG17" s="16"/>
+      <c r="FH17" s="16"/>
+      <c r="FI17" s="16"/>
+      <c r="FJ17" s="16"/>
+      <c r="FK17" s="16"/>
+      <c r="FL17" s="16"/>
+      <c r="FM17" s="16"/>
+      <c r="FN17" s="16"/>
+      <c r="FO17" s="16"/>
+      <c r="FP17" s="16"/>
+      <c r="FQ17" s="16"/>
+      <c r="FR17" s="16"/>
+      <c r="FS17" s="16"/>
+      <c r="FT17" s="16"/>
+      <c r="FU17" s="16"/>
+      <c r="FV17" s="16"/>
+      <c r="FW17" s="16"/>
+      <c r="FX17" s="16"/>
+      <c r="FY17" s="16"/>
+      <c r="FZ17" s="16"/>
+      <c r="GA17" s="16"/>
+      <c r="GB17" s="16"/>
+      <c r="GC17" s="16"/>
+      <c r="GD17" s="16"/>
+      <c r="GE17" s="16"/>
+      <c r="GF17" s="16"/>
+      <c r="GG17" s="16"/>
+      <c r="GH17" s="16"/>
+      <c r="GI17" s="16"/>
+      <c r="GJ17" s="16"/>
+      <c r="GK17" s="16"/>
+      <c r="GL17" s="16"/>
+      <c r="GM17" s="16"/>
+      <c r="GN17" s="16"/>
+      <c r="GO17" s="16"/>
+      <c r="GP17" s="16"/>
+      <c r="GQ17" s="16"/>
+      <c r="GR17" s="16"/>
+      <c r="GS17" s="16"/>
+      <c r="GT17" s="16"/>
+      <c r="GU17" s="16"/>
+      <c r="GV17" s="16"/>
+      <c r="GW17" s="16"/>
+      <c r="GX17" s="16"/>
+      <c r="GY17" s="16"/>
+      <c r="GZ17" s="16"/>
+      <c r="HA17" s="16"/>
+      <c r="HB17" s="16"/>
+      <c r="HC17" s="16"/>
+      <c r="HD17" s="16"/>
+      <c r="HE17" s="16"/>
+      <c r="HF17" s="16"/>
+      <c r="HG17" s="16"/>
+      <c r="HH17" s="16"/>
+      <c r="HI17" s="16"/>
+      <c r="HJ17" s="16"/>
+      <c r="HK17" s="16"/>
+      <c r="HL17" s="16"/>
+      <c r="HM17" s="16"/>
+      <c r="HN17" s="16"/>
+      <c r="HO17" s="16"/>
+      <c r="HP17" s="16"/>
+      <c r="HQ17" s="16"/>
+      <c r="HR17" s="16"/>
+      <c r="HS17" s="16"/>
+      <c r="HT17" s="16"/>
+      <c r="HU17" s="16"/>
+      <c r="HV17" s="16"/>
+      <c r="HW17" s="16"/>
+      <c r="HX17" s="16"/>
+      <c r="HY17" s="16"/>
+      <c r="HZ17" s="16"/>
+      <c r="IA17" s="16"/>
+      <c r="IB17" s="16"/>
+      <c r="IC17" s="16"/>
+      <c r="ID17" s="16"/>
+      <c r="IE17" s="16"/>
+      <c r="IF17" s="16"/>
+      <c r="IG17" s="16"/>
+      <c r="IH17" s="16"/>
+      <c r="II17" s="16"/>
+      <c r="IJ17" s="16"/>
+      <c r="IK17" s="16"/>
+      <c r="IL17" s="16"/>
+      <c r="IM17" s="16"/>
+      <c r="IN17" s="16"/>
+      <c r="IO17" s="16"/>
+      <c r="IP17" s="16"/>
+      <c r="IQ17" s="16"/>
+      <c r="IR17" s="16"/>
+      <c r="IS17" s="16"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
-        <v>373</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>374</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
     </row>
     <row r="20" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E20" s="25"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E21" s="21"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.511805555555555" footer="0.25"/>

</xml_diff>

<commit_message>
Add new languages to initial_date
</commit_message>
<xml_diff>
--- a/trans/initial_data/initial_data.xlsx
+++ b/trans/initial_data/initial_data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="382">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -208,6 +208,9 @@
     <t xml:space="preserve">IDN</t>
   </si>
   <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
     <t xml:space="preserve">IRN</t>
   </si>
   <si>
@@ -379,675 +382,675 @@
     <t xml:space="preserve">THA</t>
   </si>
   <si>
+    <t xml:space="preserve">TUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TKM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UZB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VNM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argentina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Austria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azerbaijan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangladesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belarus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belgium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolivia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bulgaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colombia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Croatia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyprus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czech Republic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dominican Republic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egypt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Salvador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Georgia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hong Kong, China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hungary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iceland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indonesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ireland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kazakhstan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyrgyzstan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latvia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithuania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luxembourg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macao, China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macedonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malaysia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moldova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mongolia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montenegro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morocco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netherlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nigeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palestine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Philippines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portugal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Republic of Korea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russian Federation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serbia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singapore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovakia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sri Lanka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switzerland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taiwan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tajikistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tunisia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkmenistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ukraine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States of America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uzbekistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vietnam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arabic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rtl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armenian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ltr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azerbaijani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belarusian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bosnian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dutch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estonian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finnish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">French</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Georgian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">German</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hebrew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">he</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hungarian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icelandic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japanese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kazakh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyrgyz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithuanian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norwegian Bokmål</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portuguese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Romanian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serbian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spanish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swedish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tajik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thai</t>
+  </si>
+  <si>
     <t xml:space="preserve">th</t>
   </si>
   <si>
-    <t xml:space="preserve">TUN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TKM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UKR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UZB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VNM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argentina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Armenia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Austria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azerbaijan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bangladesh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belarus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belgium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bolivia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bosnia and Herzegovina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bulgaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colombia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Croatia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyprus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Czech Republic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denmark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dominican Republic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Egypt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El Salvador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Georgia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Germany</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hong Kong, China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hungary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iceland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indonesia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ireland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Italy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jordan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kazakhstan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kyrgyzstan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latvia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lithuania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luxembourg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macao, China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macedonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malaysia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mexico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moldova</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mongolia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Montenegro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morocco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Netherlands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nigeria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Norway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palestine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Philippines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portugal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Republic of Korea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Romania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Russian Federation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serbia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Singapore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slovakia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slovenia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sri Lanka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sweden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switzerland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taiwan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tajikistan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thailand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tunisia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turkey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turkmenistan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ukraine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States of America</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uzbekistan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vietnam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arabic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rtl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Armenian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ltr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azerbaijani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belarusian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bosnian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chinese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Czech</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dutch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estonian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finnish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">French</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Georgian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">German</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hebrew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">he</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hungarian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Icelandic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Italian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japanese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kazakh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kyrgyz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lithuanian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Norwegian Bokmål</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portuguese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Romanian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Russian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serbian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slovak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slovene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spanish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swedish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tajik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thai</t>
-  </si>
-  <si>
     <t xml:space="preserve">Turkish</t>
   </si>
   <si>
@@ -1061,6 +1064,9 @@
   </si>
   <si>
     <t xml:space="preserve">Korean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indonesian</t>
   </si>
   <si>
     <t xml:space="preserve">This sheet contains data imported separately by command loaddata, and is not used by command initialize.</t>
@@ -1507,8 +1513,8 @@
   </sheetPr>
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D63" activeCellId="0" sqref="D63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1946,7 +1952,7 @@
         <v>52</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>6</v>
@@ -2030,7 +2036,7 @@
         <v>60</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>6</v>
@@ -2038,13 +2044,13 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>6</v>
@@ -2052,10 +2058,10 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>10</v>
@@ -2066,13 +2072,13 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>6</v>
@@ -2080,13 +2086,13 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>6</v>
@@ -2094,10 +2100,10 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>10</v>
@@ -2108,13 +2114,13 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>6</v>
@@ -2122,13 +2128,13 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>6</v>
@@ -2136,10 +2142,10 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>10</v>
@@ -2150,13 +2156,13 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>6</v>
@@ -2164,10 +2170,10 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>12</v>
@@ -2178,10 +2184,10 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>27</v>
@@ -2192,10 +2198,10 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>10</v>
@@ -2206,10 +2212,10 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>10</v>
@@ -2220,10 +2226,10 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>5</v>
@@ -2234,10 +2240,10 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>10</v>
@@ -2248,10 +2254,10 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>10</v>
@@ -2262,10 +2268,10 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>10</v>
@@ -2276,10 +2282,10 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>43</v>
@@ -2290,10 +2296,10 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>10</v>
@@ -2304,10 +2310,10 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>10</v>
@@ -2318,13 +2324,13 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>6</v>
@@ -2332,10 +2338,10 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>43</v>
@@ -2346,10 +2352,10 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>10</v>
@@ -2360,13 +2366,13 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>6</v>
@@ -2374,10 +2380,10 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>10</v>
@@ -2388,13 +2394,13 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>6</v>
@@ -2402,13 +2408,13 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>6</v>
@@ -2416,13 +2422,13 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>6</v>
@@ -2430,13 +2436,13 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>6</v>
@@ -2444,10 +2450,10 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>10</v>
@@ -2458,13 +2464,13 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>6</v>
@@ -2472,13 +2478,13 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>6</v>
@@ -2486,10 +2492,10 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>10</v>
@@ -2500,10 +2506,10 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>5</v>
@@ -2514,10 +2520,10 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>10</v>
@@ -2528,13 +2534,13 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>6</v>
@@ -2542,13 +2548,13 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>6</v>
@@ -2556,10 +2562,10 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>43</v>
@@ -2570,10 +2576,10 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>32</v>
@@ -2584,13 +2590,13 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>6</v>
@@ -2598,13 +2604,13 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>6</v>
@@ -3406,7 +3412,7 @@
         <v>203</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>204</v>
@@ -3417,7 +3423,7 @@
         <v>205</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>206</v>
@@ -3428,7 +3434,7 @@
         <v>207</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>208</v>
@@ -3439,7 +3445,7 @@
         <v>209</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>210</v>
@@ -3450,7 +3456,7 @@
         <v>211</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>212</v>
@@ -3461,7 +3467,7 @@
         <v>213</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>214</v>
@@ -3472,7 +3478,7 @@
         <v>215</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>216</v>
@@ -3483,7 +3489,7 @@
         <v>217</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>218</v>
@@ -3494,7 +3500,7 @@
         <v>219</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>220</v>
@@ -3505,7 +3511,7 @@
         <v>221</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>222</v>
@@ -3516,7 +3522,7 @@
         <v>223</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>224</v>
@@ -3527,7 +3533,7 @@
         <v>225</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>226</v>
@@ -3538,7 +3544,7 @@
         <v>227</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>228</v>
@@ -3549,7 +3555,7 @@
         <v>229</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>230</v>
@@ -3560,7 +3566,7 @@
         <v>231</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>232</v>
@@ -3571,7 +3577,7 @@
         <v>233</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>234</v>
@@ -3582,7 +3588,7 @@
         <v>235</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>236</v>
@@ -3593,7 +3599,7 @@
         <v>237</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>238</v>
@@ -3604,7 +3610,7 @@
         <v>239</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>240</v>
@@ -3615,7 +3621,7 @@
         <v>241</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>242</v>
@@ -3626,7 +3632,7 @@
         <v>243</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>244</v>
@@ -3637,7 +3643,7 @@
         <v>245</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>246</v>
@@ -3648,7 +3654,7 @@
         <v>247</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>248</v>
@@ -3659,7 +3665,7 @@
         <v>249</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>250</v>
@@ -3670,7 +3676,7 @@
         <v>251</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>252</v>
@@ -3681,7 +3687,7 @@
         <v>253</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>254</v>
@@ -3692,7 +3698,7 @@
         <v>255</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>256</v>
@@ -3703,7 +3709,7 @@
         <v>257</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>258</v>
@@ -3714,7 +3720,7 @@
         <v>259</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>260</v>
@@ -3725,7 +3731,7 @@
         <v>261</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>262</v>
@@ -3736,7 +3742,7 @@
         <v>263</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>264</v>
@@ -3747,7 +3753,7 @@
         <v>265</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>266</v>
@@ -3758,7 +3764,7 @@
         <v>267</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>268</v>
@@ -3769,7 +3775,7 @@
         <v>269</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>270</v>
@@ -3780,7 +3786,7 @@
         <v>271</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>272</v>
@@ -3791,7 +3797,7 @@
         <v>273</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>274</v>
@@ -3802,7 +3808,7 @@
         <v>275</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>276</v>
@@ -3813,7 +3819,7 @@
         <v>277</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>278</v>
@@ -3824,7 +3830,7 @@
         <v>279</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>280</v>
@@ -3835,7 +3841,7 @@
         <v>281</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>282</v>
@@ -3846,7 +3852,7 @@
         <v>283</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>284</v>
@@ -3959,10 +3965,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:IV42"/>
+  <dimension ref="A1:IV43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4441,7 +4447,7 @@
         <v>323</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>305</v>
@@ -4452,7 +4458,7 @@
         <v>324</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>305</v>
@@ -4463,7 +4469,7 @@
         <v>325</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>305</v>
@@ -4474,7 +4480,7 @@
         <v>326</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>305</v>
@@ -4485,7 +4491,7 @@
         <v>327</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>305</v>
@@ -4496,7 +4502,7 @@
         <v>328</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>305</v>
@@ -4507,7 +4513,7 @@
         <v>329</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>303</v>
@@ -4518,7 +4524,7 @@
         <v>330</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>305</v>
@@ -4540,7 +4546,7 @@
         <v>332</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>305</v>
@@ -4551,7 +4557,7 @@
         <v>333</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>305</v>
@@ -4562,7 +4568,7 @@
         <v>334</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>305</v>
@@ -4573,7 +4579,7 @@
         <v>335</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>305</v>
@@ -4584,7 +4590,7 @@
         <v>336</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>305</v>
@@ -4606,7 +4612,7 @@
         <v>338</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>305</v>
@@ -4617,7 +4623,7 @@
         <v>339</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>305</v>
@@ -4628,7 +4634,7 @@
         <v>340</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>118</v>
+        <v>341</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>305</v>
@@ -4636,7 +4642,7 @@
     </row>
     <row r="38" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>121</v>
@@ -4647,7 +4653,7 @@
     </row>
     <row r="39" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>123</v>
@@ -4658,7 +4664,7 @@
     </row>
     <row r="40" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>125</v>
@@ -4669,7 +4675,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>129</v>
@@ -4680,12 +4686,23 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>305</v>
       </c>
     </row>
@@ -4722,7 +4739,7 @@
   <sheetData>
     <row r="1" s="12" customFormat="true" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -4979,13 +4996,13 @@
     </row>
     <row r="2" s="15" customFormat="true" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -5238,7 +5255,7 @@
     </row>
     <row r="3" s="18" customFormat="true" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>131</v>
@@ -5248,7 +5265,7 @@
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="16" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>131</v>
@@ -5513,10 +5530,10 @@
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="4" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5524,26 +5541,26 @@
         <v>329</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>303</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="4" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D6" s="19"/>
       <c r="E6" s="4" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5551,13 +5568,13 @@
     </row>
     <row r="8" s="15" customFormat="true" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="20" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -5817,22 +5834,22 @@
         <v>0</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="16"/>
@@ -6083,26 +6100,26 @@
     </row>
     <row r="10" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="24" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="G10" s="25" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -6114,26 +6131,26 @@
     </row>
     <row r="11" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="24" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="G11" s="25" t="n">
         <v>1</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -6145,20 +6162,20 @@
     </row>
     <row r="12" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="24" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="G12" s="25" t="n">
         <v>2</v>
@@ -6177,26 +6194,26 @@
     </row>
     <row r="13" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="24" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="G13" s="25" t="n">
         <v>3</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -6208,26 +6225,26 @@
     </row>
     <row r="14" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="24" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="G14" s="25" t="n">
         <v>4</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -6250,7 +6267,7 @@
     </row>
     <row r="16" s="15" customFormat="true" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -6507,10 +6524,10 @@
     </row>
     <row r="17" s="18" customFormat="true" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -6766,10 +6783,10 @@
     </row>
     <row r="18" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>

</xml_diff>